<commit_message>
dump dataset BASE values , too
</commit_message>
<xml_diff>
--- a/TestSet21.xlsx
+++ b/TestSet21.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'21-Scripts'!$A$4:$S$88</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'21-Scripts'!$A$4:$T$88</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="49">
   <si>
     <t>SCGD</t>
   </si>
@@ -173,6 +173,9 @@
   </si>
   <si>
     <t>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0a-bsc1.xml Config.NoInclude/Engines/SCGD-1-1.xml 5920</t>
+  </si>
+  <si>
+    <t>OOS Infer Dataset</t>
   </si>
 </sst>
 </file>
@@ -642,13 +645,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:S93"/>
+  <dimension ref="A1:T93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="64" topLeftCell="G65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="64" topLeftCell="F65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A65" sqref="A65"/>
-      <selection pane="bottomRight" activeCell="J68" sqref="J68"/>
+      <selection pane="bottomRight" activeCell="J75" sqref="J75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,61 +666,65 @@
     <col min="8" max="8" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="35.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.5703125" customWidth="1"/>
-    <col min="11" max="11" width="32.28515625" customWidth="1"/>
-    <col min="12" max="16" width="32" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.28515625" customWidth="1"/>
+    <col min="13" max="17" width="32" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="34.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O1" s="2"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>21</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="T2" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K3" s="4"/>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
-    </row>
-    <row r="4" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q3" s="4"/>
+    </row>
+    <row r="4" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -748,44 +755,44 @@
       <c r="J4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="2" t="str">
-        <f>RIGHT(K2,LEN(K2)-26)</f>
+      <c r="L4" s="2" t="str">
+        <f>RIGHT(L2,LEN(L2)-26)</f>
         <v>i0.xml</v>
       </c>
-      <c r="L4" s="2" t="str">
-        <f t="shared" ref="L4:S4" si="0">RIGHT(L2,LEN(L2)-26)</f>
+      <c r="M4" s="2" t="str">
+        <f t="shared" ref="M4:T4" si="0">RIGHT(M2,LEN(M2)-26)</f>
         <v>i1.xml</v>
       </c>
-      <c r="M4" s="2" t="str">
+      <c r="N4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>i2.xml</v>
       </c>
-      <c r="N4" s="2" t="str">
+      <c r="O4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>i0a.xml</v>
       </c>
-      <c r="O4" s="2" t="str">
+      <c r="P4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>i0b.xml</v>
       </c>
-      <c r="P4" s="2" t="str">
+      <c r="Q4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>i0c.xml</v>
       </c>
-      <c r="Q4" s="2" t="str">
+      <c r="R4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>i0a-bsc1.xml</v>
       </c>
-      <c r="R4" s="2" t="str">
+      <c r="S4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>i0b-bsc1.xml</v>
       </c>
-      <c r="S4" s="2" t="str">
+      <c r="T4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>i0c-bsc1.xml</v>
       </c>
     </row>
-    <row r="5" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6556</v>
       </c>
@@ -821,32 +828,32 @@
         <f t="shared" ref="J5:J36" si="5">"zzz Both "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;G5&amp;" "&amp;I5&amp;" "&amp;H5</f>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/STD-2.xml</v>
       </c>
-      <c r="K5" t="str">
-        <f t="shared" ref="K5:P20" si="6">"zzz Infer "&amp;$A$2&amp;" "&amp;$F5&amp;" "&amp;K$2&amp;" "&amp;$A5</f>
+      <c r="L5" t="str">
+        <f t="shared" ref="L5:Q20" si="6">"zzz Infer "&amp;$A$2&amp;" "&amp;$F5&amp;" "&amp;L$2&amp;" "&amp;$A5</f>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 6556</v>
       </c>
-      <c r="L5" t="str">
+      <c r="M5" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 6556</v>
       </c>
-      <c r="M5" t="str">
+      <c r="N5" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 6556</v>
       </c>
-      <c r="N5" t="str">
+      <c r="O5" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 6556</v>
       </c>
-      <c r="O5" t="str">
+      <c r="P5" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 6556</v>
       </c>
-      <c r="P5" t="str">
+      <c r="Q5" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 6556</v>
       </c>
     </row>
-    <row r="6" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>9048</v>
       </c>
@@ -882,32 +889,32 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/STD-2.xml</v>
       </c>
-      <c r="K6" t="str">
+      <c r="L6" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 9048</v>
       </c>
-      <c r="L6" t="str">
+      <c r="M6" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 9048</v>
       </c>
-      <c r="M6" t="str">
+      <c r="N6" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 9048</v>
       </c>
-      <c r="N6" t="str">
+      <c r="O6" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 9048</v>
       </c>
-      <c r="O6" t="str">
+      <c r="P6" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 9048</v>
       </c>
-      <c r="P6" t="str">
+      <c r="Q6" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 9048</v>
       </c>
     </row>
-    <row r="7" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>5368</v>
       </c>
@@ -943,35 +950,36 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/STD-2.xml</v>
       </c>
-      <c r="K7" t="str">
+      <c r="K7" s="13"/>
+      <c r="L7" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 5368</v>
       </c>
-      <c r="L7" t="str">
+      <c r="M7" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 5368</v>
       </c>
-      <c r="M7" t="str">
+      <c r="N7" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 5368</v>
       </c>
-      <c r="N7" t="str">
+      <c r="O7" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 5368</v>
       </c>
-      <c r="O7" t="str">
+      <c r="P7" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 5368</v>
       </c>
-      <c r="P7" t="str">
+      <c r="Q7" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 5368</v>
       </c>
-      <c r="Q7" s="13"/>
       <c r="R7" s="13"/>
       <c r="S7" s="13"/>
-    </row>
-    <row r="8" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="T7" s="13"/>
+    </row>
+    <row r="8" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1624</v>
       </c>
@@ -1007,32 +1015,32 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/STD-2.xml</v>
       </c>
-      <c r="K8" t="str">
+      <c r="L8" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 1624</v>
       </c>
-      <c r="L8" t="str">
+      <c r="M8" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 1624</v>
       </c>
-      <c r="M8" t="str">
+      <c r="N8" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 1624</v>
       </c>
-      <c r="N8" t="str">
+      <c r="O8" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 1624</v>
       </c>
-      <c r="O8" t="str">
+      <c r="P8" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 1624</v>
       </c>
-      <c r="P8" t="str">
+      <c r="Q8" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 1624</v>
       </c>
     </row>
-    <row r="9" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9368</v>
       </c>
@@ -1068,32 +1076,32 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/STD-2.xml</v>
       </c>
-      <c r="K9" t="str">
+      <c r="L9" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 9368</v>
       </c>
-      <c r="L9" t="str">
+      <c r="M9" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 9368</v>
       </c>
-      <c r="M9" t="str">
+      <c r="N9" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 9368</v>
       </c>
-      <c r="N9" t="str">
+      <c r="O9" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 9368</v>
       </c>
-      <c r="O9" t="str">
+      <c r="P9" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 9368</v>
       </c>
-      <c r="P9" t="str">
+      <c r="Q9" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 9368</v>
       </c>
     </row>
-    <row r="10" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3400</v>
       </c>
@@ -1129,32 +1137,32 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/STD-2.xml</v>
       </c>
-      <c r="K10" t="str">
+      <c r="L10" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 3400</v>
       </c>
-      <c r="L10" t="str">
+      <c r="M10" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 3400</v>
       </c>
-      <c r="M10" t="str">
+      <c r="N10" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 3400</v>
       </c>
-      <c r="N10" t="str">
+      <c r="O10" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 3400</v>
       </c>
-      <c r="O10" t="str">
+      <c r="P10" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 3400</v>
       </c>
-      <c r="P10" t="str">
+      <c r="Q10" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 3400</v>
       </c>
     </row>
-    <row r="11" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9372</v>
       </c>
@@ -1190,32 +1198,32 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/STD-2.xml</v>
       </c>
-      <c r="K11" t="str">
+      <c r="L11" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 9372</v>
       </c>
-      <c r="L11" t="str">
+      <c r="M11" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 9372</v>
       </c>
-      <c r="M11" t="str">
+      <c r="N11" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 9372</v>
       </c>
-      <c r="N11" t="str">
+      <c r="O11" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 9372</v>
       </c>
-      <c r="O11" t="str">
+      <c r="P11" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 9372</v>
       </c>
-      <c r="P11" t="str">
+      <c r="Q11" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 9372</v>
       </c>
     </row>
-    <row r="12" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3576</v>
       </c>
@@ -1251,32 +1259,32 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/STD-2.xml</v>
       </c>
-      <c r="K12" t="str">
+      <c r="L12" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 3576</v>
       </c>
-      <c r="L12" t="str">
+      <c r="M12" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 3576</v>
       </c>
-      <c r="M12" t="str">
+      <c r="N12" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 3576</v>
       </c>
-      <c r="N12" t="str">
+      <c r="O12" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 3576</v>
       </c>
-      <c r="O12" t="str">
+      <c r="P12" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 3576</v>
       </c>
-      <c r="P12" t="str">
+      <c r="Q12" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 3576</v>
       </c>
     </row>
-    <row r="13" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1980</v>
       </c>
@@ -1312,32 +1320,32 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/STD-2.xml</v>
       </c>
-      <c r="K13" t="str">
+      <c r="L13" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 1980</v>
       </c>
-      <c r="L13" t="str">
+      <c r="M13" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 1980</v>
       </c>
-      <c r="M13" t="str">
+      <c r="N13" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 1980</v>
       </c>
-      <c r="N13" t="str">
+      <c r="O13" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 1980</v>
       </c>
-      <c r="O13" t="str">
+      <c r="P13" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 1980</v>
       </c>
-      <c r="P13" t="str">
+      <c r="Q13" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 1980</v>
       </c>
     </row>
-    <row r="14" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>8052</v>
       </c>
@@ -1373,32 +1381,32 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/STD-2.xml</v>
       </c>
-      <c r="K14" t="str">
+      <c r="L14" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 8052</v>
       </c>
-      <c r="L14" t="str">
+      <c r="M14" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 8052</v>
       </c>
-      <c r="M14" t="str">
+      <c r="N14" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 8052</v>
       </c>
-      <c r="N14" t="str">
+      <c r="O14" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 8052</v>
       </c>
-      <c r="O14" t="str">
+      <c r="P14" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 8052</v>
       </c>
-      <c r="P14" t="str">
+      <c r="Q14" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 8052</v>
       </c>
     </row>
-    <row r="15" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>5532</v>
       </c>
@@ -1434,32 +1442,32 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/STD-2.xml</v>
       </c>
-      <c r="K15" t="str">
+      <c r="L15" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 5532</v>
       </c>
-      <c r="L15" t="str">
+      <c r="M15" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 5532</v>
       </c>
-      <c r="M15" t="str">
+      <c r="N15" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 5532</v>
       </c>
-      <c r="N15" t="str">
+      <c r="O15" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 5532</v>
       </c>
-      <c r="O15" t="str">
+      <c r="P15" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 5532</v>
       </c>
-      <c r="P15" t="str">
+      <c r="Q15" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 5532</v>
       </c>
     </row>
-    <row r="16" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>6348</v>
       </c>
@@ -1495,32 +1503,32 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/STD-2.xml</v>
       </c>
-      <c r="K16" t="str">
+      <c r="L16" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 6348</v>
       </c>
-      <c r="L16" t="str">
+      <c r="M16" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 6348</v>
       </c>
-      <c r="M16" t="str">
+      <c r="N16" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 6348</v>
       </c>
-      <c r="N16" t="str">
+      <c r="O16" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 6348</v>
       </c>
-      <c r="O16" t="str">
+      <c r="P16" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 6348</v>
       </c>
-      <c r="P16" t="str">
+      <c r="Q16" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 6348</v>
       </c>
     </row>
-    <row r="17" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>9488</v>
       </c>
@@ -1556,32 +1564,32 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/STD-1-1.xml</v>
       </c>
-      <c r="K17" t="str">
+      <c r="L17" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 9488</v>
       </c>
-      <c r="L17" t="str">
+      <c r="M17" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 9488</v>
       </c>
-      <c r="M17" t="str">
+      <c r="N17" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 9488</v>
       </c>
-      <c r="N17" t="str">
+      <c r="O17" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 9488</v>
       </c>
-      <c r="O17" t="str">
+      <c r="P17" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 9488</v>
       </c>
-      <c r="P17" t="str">
+      <c r="Q17" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 9488</v>
       </c>
     </row>
-    <row r="18" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4616</v>
       </c>
@@ -1617,32 +1625,32 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/STD-1-1.xml</v>
       </c>
-      <c r="K18" t="str">
+      <c r="L18" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 4616</v>
       </c>
-      <c r="L18" t="str">
+      <c r="M18" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 4616</v>
       </c>
-      <c r="M18" t="str">
+      <c r="N18" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 4616</v>
       </c>
-      <c r="N18" t="str">
+      <c r="O18" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 4616</v>
       </c>
-      <c r="O18" t="str">
+      <c r="P18" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 4616</v>
       </c>
-      <c r="P18" t="str">
+      <c r="Q18" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 4616</v>
       </c>
     </row>
-    <row r="19" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>7656</v>
       </c>
@@ -1678,32 +1686,32 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/STD-1-1.xml</v>
       </c>
-      <c r="K19" t="str">
+      <c r="L19" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 7656</v>
       </c>
-      <c r="L19" t="str">
+      <c r="M19" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 7656</v>
       </c>
-      <c r="M19" t="str">
+      <c r="N19" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 7656</v>
       </c>
-      <c r="N19" t="str">
+      <c r="O19" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 7656</v>
       </c>
-      <c r="O19" t="str">
+      <c r="P19" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 7656</v>
       </c>
-      <c r="P19" t="str">
+      <c r="Q19" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 7656</v>
       </c>
     </row>
-    <row r="20" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5340</v>
       </c>
@@ -1739,32 +1747,32 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/STD-1-1.xml</v>
       </c>
-      <c r="K20" t="str">
+      <c r="L20" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 5340</v>
       </c>
-      <c r="L20" t="str">
+      <c r="M20" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 5340</v>
       </c>
-      <c r="M20" t="str">
+      <c r="N20" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 5340</v>
       </c>
-      <c r="N20" t="str">
+      <c r="O20" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 5340</v>
       </c>
-      <c r="O20" t="str">
+      <c r="P20" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 5340</v>
       </c>
-      <c r="P20" t="str">
+      <c r="Q20" t="str">
         <f t="shared" si="6"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 5340</v>
       </c>
     </row>
-    <row r="21" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>9312</v>
       </c>
@@ -1800,32 +1808,32 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/STD-1-1.xml</v>
       </c>
-      <c r="K21" t="str">
-        <f t="shared" ref="K21:P36" si="7">"zzz Infer "&amp;$A$2&amp;" "&amp;$F21&amp;" "&amp;K$2&amp;" "&amp;$A21</f>
+      <c r="L21" t="str">
+        <f t="shared" ref="L21:Q36" si="7">"zzz Infer "&amp;$A$2&amp;" "&amp;$F21&amp;" "&amp;L$2&amp;" "&amp;$A21</f>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 9312</v>
       </c>
-      <c r="L21" t="str">
+      <c r="M21" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 9312</v>
       </c>
-      <c r="M21" t="str">
+      <c r="N21" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 9312</v>
       </c>
-      <c r="N21" t="str">
+      <c r="O21" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 9312</v>
       </c>
-      <c r="O21" t="str">
+      <c r="P21" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 9312</v>
       </c>
-      <c r="P21" t="str">
+      <c r="Q21" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 9312</v>
       </c>
     </row>
-    <row r="22" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3144</v>
       </c>
@@ -1861,32 +1869,32 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/STD-1-1.xml</v>
       </c>
-      <c r="K22" t="str">
+      <c r="L22" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 3144</v>
       </c>
-      <c r="L22" t="str">
+      <c r="M22" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 3144</v>
       </c>
-      <c r="M22" t="str">
+      <c r="N22" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 3144</v>
       </c>
-      <c r="N22" t="str">
+      <c r="O22" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 3144</v>
       </c>
-      <c r="O22" t="str">
+      <c r="P22" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 3144</v>
       </c>
-      <c r="P22" t="str">
+      <c r="Q22" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 3144</v>
       </c>
     </row>
-    <row r="23" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>7688</v>
       </c>
@@ -1922,32 +1930,32 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/STD-1-1.xml</v>
       </c>
-      <c r="K23" t="str">
+      <c r="L23" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 7688</v>
       </c>
-      <c r="L23" t="str">
+      <c r="M23" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 7688</v>
       </c>
-      <c r="M23" t="str">
+      <c r="N23" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 7688</v>
       </c>
-      <c r="N23" t="str">
+      <c r="O23" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 7688</v>
       </c>
-      <c r="O23" t="str">
+      <c r="P23" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 7688</v>
       </c>
-      <c r="P23" t="str">
+      <c r="Q23" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 7688</v>
       </c>
     </row>
-    <row r="24" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3780</v>
       </c>
@@ -1983,32 +1991,32 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/STD-1-1.xml</v>
       </c>
-      <c r="K24" t="str">
+      <c r="L24" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 3780</v>
       </c>
-      <c r="L24" t="str">
+      <c r="M24" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 3780</v>
       </c>
-      <c r="M24" t="str">
+      <c r="N24" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 3780</v>
       </c>
-      <c r="N24" t="str">
+      <c r="O24" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 3780</v>
       </c>
-      <c r="O24" t="str">
+      <c r="P24" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 3780</v>
       </c>
-      <c r="P24" t="str">
+      <c r="Q24" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 3780</v>
       </c>
     </row>
-    <row r="25" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>796</v>
       </c>
@@ -2044,32 +2052,32 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/STD-1-1.xml</v>
       </c>
-      <c r="K25" t="str">
+      <c r="L25" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 796</v>
       </c>
-      <c r="L25" t="str">
+      <c r="M25" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 796</v>
       </c>
-      <c r="M25" t="str">
+      <c r="N25" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 796</v>
       </c>
-      <c r="N25" t="str">
+      <c r="O25" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 796</v>
       </c>
-      <c r="O25" t="str">
+      <c r="P25" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 796</v>
       </c>
-      <c r="P25" t="str">
+      <c r="Q25" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 796</v>
       </c>
     </row>
-    <row r="26" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1340</v>
       </c>
@@ -2105,32 +2113,32 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/STD-1-1.xml</v>
       </c>
-      <c r="K26" t="str">
+      <c r="L26" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 1340</v>
       </c>
-      <c r="L26" t="str">
+      <c r="M26" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 1340</v>
       </c>
-      <c r="M26" t="str">
+      <c r="N26" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 1340</v>
       </c>
-      <c r="N26" t="str">
+      <c r="O26" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 1340</v>
       </c>
-      <c r="O26" t="str">
+      <c r="P26" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 1340</v>
       </c>
-      <c r="P26" t="str">
+      <c r="Q26" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 1340</v>
       </c>
     </row>
-    <row r="27" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>8896</v>
       </c>
@@ -2166,32 +2174,32 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/STD-1-1.xml</v>
       </c>
-      <c r="K27" t="str">
+      <c r="L27" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 8896</v>
       </c>
-      <c r="L27" t="str">
+      <c r="M27" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 8896</v>
       </c>
-      <c r="M27" t="str">
+      <c r="N27" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 8896</v>
       </c>
-      <c r="N27" t="str">
+      <c r="O27" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 8896</v>
       </c>
-      <c r="O27" t="str">
+      <c r="P27" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 8896</v>
       </c>
-      <c r="P27" t="str">
+      <c r="Q27" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 8896</v>
       </c>
     </row>
-    <row r="28" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>5656</v>
       </c>
@@ -2227,32 +2235,32 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/STD-1-1.xml</v>
       </c>
-      <c r="K28" t="str">
+      <c r="L28" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 5656</v>
       </c>
-      <c r="L28" t="str">
+      <c r="M28" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 5656</v>
       </c>
-      <c r="M28" t="str">
+      <c r="N28" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 5656</v>
       </c>
-      <c r="N28" t="str">
+      <c r="O28" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 5656</v>
       </c>
-      <c r="O28" t="str">
+      <c r="P28" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 5656</v>
       </c>
-      <c r="P28" t="str">
+      <c r="Q28" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 5656</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>2416</v>
       </c>
@@ -2288,32 +2296,33 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/STD-2-2-1.xml</v>
       </c>
-      <c r="K29" t="str">
+      <c r="K29" s="13"/>
+      <c r="L29" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 2416</v>
       </c>
-      <c r="L29" t="str">
+      <c r="M29" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 2416</v>
       </c>
-      <c r="M29" t="str">
+      <c r="N29" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 2416</v>
       </c>
-      <c r="N29" t="str">
+      <c r="O29" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 2416</v>
       </c>
-      <c r="O29" t="str">
+      <c r="P29" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 2416</v>
       </c>
-      <c r="P29" t="str">
+      <c r="Q29" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 2416</v>
       </c>
     </row>
-    <row r="30" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>4696</v>
       </c>
@@ -2349,32 +2358,32 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/STD-2-2-1.xml</v>
       </c>
-      <c r="K30" t="str">
+      <c r="L30" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 4696</v>
       </c>
-      <c r="L30" t="str">
+      <c r="M30" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 4696</v>
       </c>
-      <c r="M30" t="str">
+      <c r="N30" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 4696</v>
       </c>
-      <c r="N30" t="str">
+      <c r="O30" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 4696</v>
       </c>
-      <c r="O30" t="str">
+      <c r="P30" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 4696</v>
       </c>
-      <c r="P30" t="str">
+      <c r="Q30" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 4696</v>
       </c>
     </row>
-    <row r="31" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>40</v>
       </c>
@@ -2410,32 +2419,32 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/STD-2-2-1.xml</v>
       </c>
-      <c r="K31" t="str">
+      <c r="L31" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml MEM!</v>
       </c>
-      <c r="L31" t="str">
+      <c r="M31" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml MEM!</v>
       </c>
-      <c r="M31" t="str">
+      <c r="N31" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml MEM!</v>
       </c>
-      <c r="N31" t="str">
+      <c r="O31" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml MEM!</v>
       </c>
-      <c r="O31" t="str">
+      <c r="P31" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml MEM!</v>
       </c>
-      <c r="P31" t="str">
+      <c r="Q31" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml MEM!</v>
       </c>
     </row>
-    <row r="32" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>7252</v>
       </c>
@@ -2471,32 +2480,32 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/STD-2-2-1.xml</v>
       </c>
-      <c r="K32" t="str">
+      <c r="L32" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 7252</v>
       </c>
-      <c r="L32" t="str">
+      <c r="M32" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 7252</v>
       </c>
-      <c r="M32" t="str">
+      <c r="N32" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 7252</v>
       </c>
-      <c r="N32" t="str">
+      <c r="O32" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 7252</v>
       </c>
-      <c r="O32" t="str">
+      <c r="P32" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 7252</v>
       </c>
-      <c r="P32" t="str">
+      <c r="Q32" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 7252</v>
       </c>
     </row>
-    <row r="33" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>4880</v>
       </c>
@@ -2532,32 +2541,32 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/STD-2-2-1.xml</v>
       </c>
-      <c r="K33" t="str">
+      <c r="L33" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 4880</v>
       </c>
-      <c r="L33" t="str">
+      <c r="M33" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 4880</v>
       </c>
-      <c r="M33" t="str">
+      <c r="N33" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 4880</v>
       </c>
-      <c r="N33" t="str">
+      <c r="O33" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 4880</v>
       </c>
-      <c r="O33" t="str">
+      <c r="P33" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 4880</v>
       </c>
-      <c r="P33" t="str">
+      <c r="Q33" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 4880</v>
       </c>
     </row>
-    <row r="34" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>40</v>
       </c>
@@ -2593,32 +2602,32 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/STD-2-2-1.xml</v>
       </c>
-      <c r="K34" t="str">
+      <c r="L34" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml MEM!</v>
       </c>
-      <c r="L34" t="str">
+      <c r="M34" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml MEM!</v>
       </c>
-      <c r="M34" t="str">
+      <c r="N34" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml MEM!</v>
       </c>
-      <c r="N34" t="str">
+      <c r="O34" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml MEM!</v>
       </c>
-      <c r="O34" t="str">
+      <c r="P34" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml MEM!</v>
       </c>
-      <c r="P34" t="str">
+      <c r="Q34" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml MEM!</v>
       </c>
     </row>
-    <row r="35" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3476</v>
       </c>
@@ -2654,32 +2663,32 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/STD-2-2-1.xml</v>
       </c>
-      <c r="K35" t="str">
+      <c r="L35" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 3476</v>
       </c>
-      <c r="L35" t="str">
+      <c r="M35" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 3476</v>
       </c>
-      <c r="M35" t="str">
+      <c r="N35" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 3476</v>
       </c>
-      <c r="N35" t="str">
+      <c r="O35" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 3476</v>
       </c>
-      <c r="O35" t="str">
+      <c r="P35" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 3476</v>
       </c>
-      <c r="P35" t="str">
+      <c r="Q35" t="str">
         <f t="shared" si="7"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 3476</v>
       </c>
     </row>
-    <row r="36" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>3</v>
       </c>
@@ -2712,32 +2721,32 @@
         <f t="shared" si="5"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/STD-2-2-1.xml</v>
       </c>
-      <c r="K36" t="str">
+      <c r="L36" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
       </c>
-      <c r="L36" t="str">
+      <c r="M36" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
       </c>
-      <c r="M36" t="str">
+      <c r="N36" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
       </c>
-      <c r="N36" t="str">
+      <c r="O36" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
       </c>
-      <c r="O36" t="str">
+      <c r="P36" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
       </c>
-      <c r="P36" t="str">
+      <c r="Q36" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="37" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>3</v>
       </c>
@@ -2770,32 +2779,32 @@
         <f t="shared" ref="J37:J68" si="12">"zzz Both "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;G37&amp;" "&amp;I37&amp;" "&amp;H37</f>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/STD-2-2-1.xml</v>
       </c>
-      <c r="K37" t="str">
-        <f t="shared" ref="K37:P52" si="13">"zzz Infer "&amp;$A$2&amp;" "&amp;$F37&amp;" "&amp;K$2&amp;" "&amp;$A37</f>
+      <c r="L37" t="str">
+        <f t="shared" ref="L37:Q52" si="13">"zzz Infer "&amp;$A$2&amp;" "&amp;$F37&amp;" "&amp;L$2&amp;" "&amp;$A37</f>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
       </c>
-      <c r="L37" t="str">
+      <c r="M37" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
       </c>
-      <c r="M37" t="str">
+      <c r="N37" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
       </c>
-      <c r="N37" t="str">
+      <c r="O37" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
       </c>
-      <c r="O37" t="str">
+      <c r="P37" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
       </c>
-      <c r="P37" t="str">
+      <c r="Q37" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="38" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>3</v>
       </c>
@@ -2828,32 +2837,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/STD-2-2-1.xml</v>
       </c>
-      <c r="K38" t="str">
+      <c r="L38" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
       </c>
-      <c r="L38" t="str">
+      <c r="M38" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
       </c>
-      <c r="M38" t="str">
+      <c r="N38" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
       </c>
-      <c r="N38" t="str">
+      <c r="O38" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
       </c>
-      <c r="O38" t="str">
+      <c r="P38" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
       </c>
-      <c r="P38" t="str">
+      <c r="Q38" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="39" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>3</v>
       </c>
@@ -2886,32 +2895,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/STD-2-2-1.xml</v>
       </c>
-      <c r="K39" t="str">
+      <c r="L39" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
       </c>
-      <c r="L39" t="str">
+      <c r="M39" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
       </c>
-      <c r="M39" t="str">
+      <c r="N39" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
       </c>
-      <c r="N39" t="str">
+      <c r="O39" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
       </c>
-      <c r="O39" t="str">
+      <c r="P39" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
       </c>
-      <c r="P39" t="str">
+      <c r="Q39" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="40" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>3</v>
       </c>
@@ -2944,32 +2953,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/STD-2-2-1.xml</v>
       </c>
-      <c r="K40" t="str">
+      <c r="L40" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
       </c>
-      <c r="L40" t="str">
+      <c r="M40" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
       </c>
-      <c r="M40" t="str">
+      <c r="N40" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
       </c>
-      <c r="N40" t="str">
+      <c r="O40" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
       </c>
-      <c r="O40" t="str">
+      <c r="P40" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
       </c>
-      <c r="P40" t="str">
+      <c r="Q40" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="41" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
         <v>5764</v>
       </c>
@@ -3005,32 +3014,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-2.xml</v>
       </c>
-      <c r="K41" t="str">
+      <c r="L41" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 5764</v>
       </c>
-      <c r="L41" t="str">
+      <c r="M41" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 5764</v>
       </c>
-      <c r="M41" t="str">
+      <c r="N41" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 5764</v>
       </c>
-      <c r="N41" t="str">
+      <c r="O41" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 5764</v>
       </c>
-      <c r="O41" t="str">
+      <c r="P41" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 5764</v>
       </c>
-      <c r="P41" t="str">
+      <c r="Q41" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 5764</v>
       </c>
     </row>
-    <row r="42" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>5648</v>
       </c>
@@ -3066,32 +3075,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-2.xml</v>
       </c>
-      <c r="K42" t="str">
+      <c r="L42" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 5648</v>
       </c>
-      <c r="L42" t="str">
+      <c r="M42" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 5648</v>
       </c>
-      <c r="M42" t="str">
+      <c r="N42" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 5648</v>
       </c>
-      <c r="N42" t="str">
+      <c r="O42" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 5648</v>
       </c>
-      <c r="O42" t="str">
+      <c r="P42" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 5648</v>
       </c>
-      <c r="P42" t="str">
+      <c r="Q42" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 5648</v>
       </c>
     </row>
-    <row r="43" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="13">
         <v>6176</v>
       </c>
@@ -3127,35 +3136,36 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-2.xml</v>
       </c>
-      <c r="K43" t="str">
+      <c r="K43" s="13"/>
+      <c r="L43" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 6176</v>
       </c>
-      <c r="L43" t="str">
+      <c r="M43" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 6176</v>
       </c>
-      <c r="M43" t="str">
+      <c r="N43" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 6176</v>
       </c>
-      <c r="N43" t="str">
+      <c r="O43" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 6176</v>
       </c>
-      <c r="O43" t="str">
+      <c r="P43" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 6176</v>
       </c>
-      <c r="P43" t="str">
+      <c r="Q43" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 6176</v>
       </c>
-      <c r="Q43" s="13"/>
       <c r="R43" s="13"/>
       <c r="S43" s="13"/>
-    </row>
-    <row r="44" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="T43" s="13"/>
+    </row>
+    <row r="44" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="B44" s="13" t="s">
         <v>0</v>
       </c>
@@ -3188,32 +3198,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/500-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-2.xml</v>
       </c>
-      <c r="K44" t="str">
+      <c r="L44" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
       </c>
-      <c r="L44" t="str">
+      <c r="M44" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
       </c>
-      <c r="M44" t="str">
+      <c r="N44" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
       </c>
-      <c r="N44" t="str">
+      <c r="O44" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
       </c>
-      <c r="O44" t="str">
+      <c r="P44" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
       </c>
-      <c r="P44" t="str">
+      <c r="Q44" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="45" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>5356</v>
       </c>
@@ -3249,32 +3259,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-2.xml</v>
       </c>
-      <c r="K45" t="str">
+      <c r="L45" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 5356</v>
       </c>
-      <c r="L45" t="str">
+      <c r="M45" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 5356</v>
       </c>
-      <c r="M45" t="str">
+      <c r="N45" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 5356</v>
       </c>
-      <c r="N45" t="str">
+      <c r="O45" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 5356</v>
       </c>
-      <c r="O45" t="str">
+      <c r="P45" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 5356</v>
       </c>
-      <c r="P45" t="str">
+      <c r="Q45" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 5356</v>
       </c>
     </row>
-    <row r="46" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>956</v>
       </c>
@@ -3310,32 +3320,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-2.xml</v>
       </c>
-      <c r="K46" t="str">
+      <c r="L46" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 956</v>
       </c>
-      <c r="L46" t="str">
+      <c r="M46" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 956</v>
       </c>
-      <c r="M46" t="str">
+      <c r="N46" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 956</v>
       </c>
-      <c r="N46" t="str">
+      <c r="O46" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 956</v>
       </c>
-      <c r="O46" t="str">
+      <c r="P46" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 956</v>
       </c>
-      <c r="P46" t="str">
+      <c r="Q46" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 956</v>
       </c>
     </row>
-    <row r="47" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>8195</v>
       </c>
@@ -3371,32 +3381,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-2.xml</v>
       </c>
-      <c r="K47" t="str">
+      <c r="L47" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 8195</v>
       </c>
-      <c r="L47" t="str">
+      <c r="M47" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 8195</v>
       </c>
-      <c r="M47" t="str">
+      <c r="N47" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 8195</v>
       </c>
-      <c r="N47" t="str">
+      <c r="O47" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 8195</v>
       </c>
-      <c r="O47" t="str">
+      <c r="P47" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 8195</v>
       </c>
-      <c r="P47" t="str">
+      <c r="Q47" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 8195</v>
       </c>
     </row>
-    <row r="48" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>0</v>
       </c>
@@ -3429,32 +3439,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/500-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-2.xml</v>
       </c>
-      <c r="K48" t="str">
+      <c r="L48" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
       </c>
-      <c r="L48" t="str">
+      <c r="M48" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
       </c>
-      <c r="M48" t="str">
+      <c r="N48" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
       </c>
-      <c r="N48" t="str">
+      <c r="O48" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
       </c>
-      <c r="O48" t="str">
+      <c r="P48" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
       </c>
-      <c r="P48" t="str">
+      <c r="Q48" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="49" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>8064</v>
       </c>
@@ -3490,32 +3500,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/SCGD-2.xml</v>
       </c>
-      <c r="K49" t="str">
+      <c r="L49" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 8064</v>
       </c>
-      <c r="L49" t="str">
+      <c r="M49" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 8064</v>
       </c>
-      <c r="M49" t="str">
+      <c r="N49" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 8064</v>
       </c>
-      <c r="N49" t="str">
+      <c r="O49" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 8064</v>
       </c>
-      <c r="O49" t="str">
+      <c r="P49" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 8064</v>
       </c>
-      <c r="P49" t="str">
+      <c r="Q49" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 8064</v>
       </c>
     </row>
-    <row r="50" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>6435</v>
       </c>
@@ -3551,32 +3561,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/SCGD-2.xml</v>
       </c>
-      <c r="K50" t="str">
+      <c r="L50" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 6435</v>
       </c>
-      <c r="L50" t="str">
+      <c r="M50" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 6435</v>
       </c>
-      <c r="M50" t="str">
+      <c r="N50" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 6435</v>
       </c>
-      <c r="N50" t="str">
+      <c r="O50" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 6435</v>
       </c>
-      <c r="O50" t="str">
+      <c r="P50" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 6435</v>
       </c>
-      <c r="P50" t="str">
+      <c r="Q50" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 6435</v>
       </c>
     </row>
-    <row r="51" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>7476</v>
       </c>
@@ -3612,32 +3622,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/SCGD-2.xml</v>
       </c>
-      <c r="K51" t="str">
+      <c r="L51" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 7476</v>
       </c>
-      <c r="L51" t="str">
+      <c r="M51" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 7476</v>
       </c>
-      <c r="M51" t="str">
+      <c r="N51" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 7476</v>
       </c>
-      <c r="N51" t="str">
+      <c r="O51" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 7476</v>
       </c>
-      <c r="O51" t="str">
+      <c r="P51" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 7476</v>
       </c>
-      <c r="P51" t="str">
+      <c r="Q51" t="str">
         <f t="shared" si="13"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 7476</v>
       </c>
     </row>
-    <row r="52" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>0</v>
       </c>
@@ -3670,32 +3680,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/500-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/SCGD-2.xml</v>
       </c>
-      <c r="K52" t="str">
+      <c r="L52" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
       </c>
-      <c r="L52" t="str">
+      <c r="M52" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
       </c>
-      <c r="M52" t="str">
+      <c r="N52" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
       </c>
-      <c r="N52" t="str">
+      <c r="O52" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
       </c>
-      <c r="O52" t="str">
+      <c r="P52" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
       </c>
-      <c r="P52" t="str">
+      <c r="Q52" t="str">
         <f t="shared" si="13"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="53" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>5212</v>
       </c>
@@ -3731,32 +3741,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/SCGD-2.xml</v>
       </c>
-      <c r="K53" t="str">
-        <f t="shared" ref="K53:P68" si="14">"zzz Infer "&amp;$A$2&amp;" "&amp;$F53&amp;" "&amp;K$2&amp;" "&amp;$A53</f>
+      <c r="L53" t="str">
+        <f t="shared" ref="L53:Q68" si="14">"zzz Infer "&amp;$A$2&amp;" "&amp;$F53&amp;" "&amp;L$2&amp;" "&amp;$A53</f>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 5212</v>
       </c>
-      <c r="L53" t="str">
+      <c r="M53" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 5212</v>
       </c>
-      <c r="M53" t="str">
+      <c r="N53" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 5212</v>
       </c>
-      <c r="N53" t="str">
+      <c r="O53" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 5212</v>
       </c>
-      <c r="O53" t="str">
+      <c r="P53" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 5212</v>
       </c>
-      <c r="P53" t="str">
+      <c r="Q53" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 5212</v>
       </c>
     </row>
-    <row r="54" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>8636</v>
       </c>
@@ -3792,32 +3802,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/SCGD-2.xml</v>
       </c>
-      <c r="K54" t="str">
+      <c r="L54" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 8636</v>
       </c>
-      <c r="L54" t="str">
+      <c r="M54" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 8636</v>
       </c>
-      <c r="M54" t="str">
+      <c r="N54" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 8636</v>
       </c>
-      <c r="N54" t="str">
+      <c r="O54" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 8636</v>
       </c>
-      <c r="O54" t="str">
+      <c r="P54" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 8636</v>
       </c>
-      <c r="P54" t="str">
+      <c r="Q54" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 8636</v>
       </c>
     </row>
-    <row r="55" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>8420</v>
       </c>
@@ -3853,32 +3863,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/SCGD-2.xml</v>
       </c>
-      <c r="K55" t="str">
+      <c r="L55" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 8420</v>
       </c>
-      <c r="L55" t="str">
+      <c r="M55" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 8420</v>
       </c>
-      <c r="M55" t="str">
+      <c r="N55" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 8420</v>
       </c>
-      <c r="N55" t="str">
+      <c r="O55" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 8420</v>
       </c>
-      <c r="O55" t="str">
+      <c r="P55" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 8420</v>
       </c>
-      <c r="P55" t="str">
+      <c r="Q55" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 8420</v>
       </c>
     </row>
-    <row r="56" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>0</v>
       </c>
@@ -3911,32 +3921,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/500-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/SCGD-2.xml</v>
       </c>
-      <c r="K56" t="str">
+      <c r="L56" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
       </c>
-      <c r="L56" t="str">
+      <c r="M56" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
       </c>
-      <c r="M56" t="str">
+      <c r="N56" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
       </c>
-      <c r="N56" t="str">
+      <c r="O56" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
       </c>
-      <c r="O56" t="str">
+      <c r="P56" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
       </c>
-      <c r="P56" t="str">
+      <c r="Q56" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="57" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
         <v>5920</v>
       </c>
@@ -3972,32 +3982,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-1-1.xml</v>
       </c>
-      <c r="K57" t="str">
+      <c r="L57" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 5920</v>
       </c>
-      <c r="L57" t="str">
+      <c r="M57" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 5920</v>
       </c>
-      <c r="M57" t="str">
+      <c r="N57" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 5920</v>
       </c>
-      <c r="N57" t="str">
+      <c r="O57" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 5920</v>
       </c>
-      <c r="O57" t="str">
+      <c r="P57" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 5920</v>
       </c>
-      <c r="P57" t="str">
+      <c r="Q57" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 5920</v>
       </c>
     </row>
-    <row r="58" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>4935</v>
       </c>
@@ -4033,32 +4043,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-1-1.xml</v>
       </c>
-      <c r="K58" t="str">
+      <c r="L58" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 4935</v>
       </c>
-      <c r="L58" t="str">
+      <c r="M58" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 4935</v>
       </c>
-      <c r="M58" t="str">
+      <c r="N58" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 4935</v>
       </c>
-      <c r="N58" t="str">
+      <c r="O58" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 4935</v>
       </c>
-      <c r="O58" t="str">
+      <c r="P58" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 4935</v>
       </c>
-      <c r="P58" t="str">
+      <c r="Q58" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 4935</v>
       </c>
     </row>
-    <row r="59" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>7360</v>
       </c>
@@ -4094,32 +4104,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-1-1.xml</v>
       </c>
-      <c r="K59" t="str">
-        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F59&amp;" "&amp;K$2&amp;" "&amp;$A59</f>
+      <c r="L59" t="str">
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F59&amp;" "&amp;L$2&amp;" "&amp;$A59</f>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 7360</v>
       </c>
-      <c r="L59" t="str">
+      <c r="M59" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 7360</v>
       </c>
-      <c r="M59" t="str">
+      <c r="N59" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 7360</v>
       </c>
-      <c r="N59" t="str">
+      <c r="O59" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 7360</v>
       </c>
-      <c r="O59" t="str">
+      <c r="P59" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 7360</v>
       </c>
-      <c r="P59" t="str">
+      <c r="Q59" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 7360</v>
       </c>
     </row>
-    <row r="60" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2444</v>
       </c>
@@ -4155,32 +4165,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/500-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-1-1.xml</v>
       </c>
-      <c r="K60" t="str">
-        <f t="shared" ref="K60:P75" si="15">"zzz Infer "&amp;$A$2&amp;" "&amp;$F60&amp;" "&amp;K$2&amp;" "&amp;$A60</f>
+      <c r="L60" t="str">
+        <f t="shared" ref="L60:Q75" si="15">"zzz Infer "&amp;$A$2&amp;" "&amp;$F60&amp;" "&amp;L$2&amp;" "&amp;$A60</f>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 2444</v>
       </c>
-      <c r="L60" t="str">
+      <c r="M60" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 2444</v>
       </c>
-      <c r="M60" t="str">
+      <c r="N60" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 2444</v>
       </c>
-      <c r="N60" t="str">
+      <c r="O60" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 2444</v>
       </c>
-      <c r="O60" t="str">
+      <c r="P60" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 2444</v>
       </c>
-      <c r="P60" t="str">
+      <c r="Q60" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 2444</v>
       </c>
     </row>
-    <row r="61" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>6307</v>
       </c>
@@ -4216,32 +4226,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-1-1.xml</v>
       </c>
-      <c r="K61" t="str">
+      <c r="L61" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 6307</v>
       </c>
-      <c r="L61" t="str">
+      <c r="M61" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 6307</v>
       </c>
-      <c r="M61" t="str">
+      <c r="N61" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 6307</v>
       </c>
-      <c r="N61" t="str">
+      <c r="O61" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 6307</v>
       </c>
-      <c r="O61" t="str">
+      <c r="P61" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 6307</v>
       </c>
-      <c r="P61" t="str">
+      <c r="Q61" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 6307</v>
       </c>
     </row>
-    <row r="62" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>6827</v>
       </c>
@@ -4277,32 +4287,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-1-1.xml</v>
       </c>
-      <c r="K62" t="str">
+      <c r="L62" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 6827</v>
       </c>
-      <c r="L62" t="str">
+      <c r="M62" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 6827</v>
       </c>
-      <c r="M62" t="str">
+      <c r="N62" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 6827</v>
       </c>
-      <c r="N62" t="str">
+      <c r="O62" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 6827</v>
       </c>
-      <c r="O62" t="str">
+      <c r="P62" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 6827</v>
       </c>
-      <c r="P62" t="str">
+      <c r="Q62" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 6827</v>
       </c>
     </row>
-    <row r="63" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>7376</v>
       </c>
@@ -4338,32 +4348,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-1-1.xml</v>
       </c>
-      <c r="K63" t="str">
+      <c r="L63" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 7376</v>
       </c>
-      <c r="L63" t="str">
+      <c r="M63" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 7376</v>
       </c>
-      <c r="M63" t="str">
+      <c r="N63" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 7376</v>
       </c>
-      <c r="N63" t="str">
+      <c r="O63" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 7376</v>
       </c>
-      <c r="O63" t="str">
+      <c r="P63" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 7376</v>
       </c>
-      <c r="P63" t="str">
+      <c r="Q63" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 7376</v>
       </c>
     </row>
-    <row r="64" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>0</v>
       </c>
@@ -4396,32 +4406,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/500-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-1-1.xml</v>
       </c>
-      <c r="K64" t="str">
+      <c r="L64" t="str">
         <f t="shared" si="15"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
       </c>
-      <c r="L64" t="str">
+      <c r="M64" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
       </c>
-      <c r="M64" t="str">
+      <c r="N64" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
       </c>
-      <c r="N64" t="str">
+      <c r="O64" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
       </c>
-      <c r="O64" t="str">
+      <c r="P64" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
       </c>
-      <c r="P64" t="str">
+      <c r="Q64" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>8892</v>
       </c>
@@ -4457,32 +4467,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/SCGD-1-1.xml</v>
       </c>
-      <c r="K65" t="str">
+      <c r="L65" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 8892</v>
       </c>
-      <c r="L65" t="str">
+      <c r="M65" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 8892</v>
       </c>
-      <c r="M65" t="str">
+      <c r="N65" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 8892</v>
       </c>
-      <c r="N65" t="str">
+      <c r="O65" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 8892</v>
       </c>
-      <c r="O65" t="str">
+      <c r="P65" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 8892</v>
       </c>
-      <c r="P65" t="str">
+      <c r="Q65" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 8892</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>6396</v>
       </c>
@@ -4518,32 +4528,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/SCGD-1-1.xml</v>
       </c>
-      <c r="K66" t="str">
+      <c r="L66" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 6396</v>
       </c>
-      <c r="L66" t="str">
+      <c r="M66" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 6396</v>
       </c>
-      <c r="M66" t="str">
+      <c r="N66" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 6396</v>
       </c>
-      <c r="N66" t="str">
+      <c r="O66" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 6396</v>
       </c>
-      <c r="O66" t="str">
+      <c r="P66" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 6396</v>
       </c>
-      <c r="P66" t="str">
+      <c r="Q66" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 6396</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>7532</v>
       </c>
@@ -4579,32 +4589,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/SCGD-1-1.xml</v>
       </c>
-      <c r="K67" t="str">
+      <c r="L67" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 7532</v>
       </c>
-      <c r="L67" t="str">
+      <c r="M67" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 7532</v>
       </c>
-      <c r="M67" t="str">
+      <c r="N67" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 7532</v>
       </c>
-      <c r="N67" t="str">
+      <c r="O67" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 7532</v>
       </c>
-      <c r="O67" t="str">
+      <c r="P67" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 7532</v>
       </c>
-      <c r="P67" t="str">
+      <c r="Q67" t="str">
         <f t="shared" si="14"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 7532</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>0</v>
       </c>
@@ -4637,32 +4647,32 @@
         <f t="shared" si="12"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/500-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/SCGD-1-1.xml</v>
       </c>
-      <c r="K68" t="str">
+      <c r="L68" t="str">
         <f t="shared" si="15"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
       </c>
-      <c r="L68" t="str">
+      <c r="M68" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
       </c>
-      <c r="M68" t="str">
+      <c r="N68" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
       </c>
-      <c r="N68" t="str">
+      <c r="O68" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
       </c>
-      <c r="O68" t="str">
+      <c r="P68" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
       </c>
-      <c r="P68" t="str">
+      <c r="Q68" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="69" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>1212</v>
       </c>
@@ -4698,32 +4708,32 @@
         <f t="shared" ref="J69:J88" si="20">"zzz Both "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;G69&amp;" "&amp;I69&amp;" "&amp;H69</f>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/SCGD-1-1.xml</v>
       </c>
-      <c r="K69" t="str">
+      <c r="L69" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 1212</v>
       </c>
-      <c r="L69" t="str">
+      <c r="M69" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 1212</v>
       </c>
-      <c r="M69" t="str">
+      <c r="N69" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 1212</v>
       </c>
-      <c r="N69" t="str">
+      <c r="O69" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 1212</v>
       </c>
-      <c r="O69" t="str">
+      <c r="P69" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 1212</v>
       </c>
-      <c r="P69" t="str">
+      <c r="Q69" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 1212</v>
       </c>
     </row>
-    <row r="70" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>5731</v>
       </c>
@@ -4759,32 +4769,32 @@
         <f t="shared" si="20"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/SCGD-1-1.xml</v>
       </c>
-      <c r="K70" t="str">
+      <c r="L70" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 5731</v>
       </c>
-      <c r="L70" t="str">
+      <c r="M70" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 5731</v>
       </c>
-      <c r="M70" t="str">
+      <c r="N70" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 5731</v>
       </c>
-      <c r="N70" t="str">
+      <c r="O70" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 5731</v>
       </c>
-      <c r="O70" t="str">
+      <c r="P70" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 5731</v>
       </c>
-      <c r="P70" t="str">
+      <c r="Q70" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 5731</v>
       </c>
     </row>
-    <row r="71" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>5892</v>
       </c>
@@ -4820,32 +4830,35 @@
         <f t="shared" si="20"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/SCGD-1-1.xml</v>
       </c>
-      <c r="K71" t="str">
+      <c r="L71" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 5892</v>
       </c>
-      <c r="L71" t="str">
+      <c r="M71" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 5892</v>
       </c>
-      <c r="M71" t="str">
+      <c r="N71" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 5892</v>
       </c>
-      <c r="N71" t="str">
+      <c r="O71" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 5892</v>
       </c>
-      <c r="O71" t="str">
+      <c r="P71" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 5892</v>
       </c>
-      <c r="P71" t="str">
+      <c r="Q71" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 5892</v>
       </c>
     </row>
-    <row r="72" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>6092</v>
+      </c>
       <c r="B72" t="s">
         <v>0</v>
       </c>
@@ -4878,32 +4891,32 @@
         <f t="shared" si="20"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/500-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/SCGD-1-1.xml</v>
       </c>
-      <c r="K72" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
-      </c>
       <c r="L72" t="str">
         <f t="shared" si="15"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 6092</v>
       </c>
       <c r="M72" t="str">
         <f t="shared" si="15"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 6092</v>
       </c>
       <c r="N72" t="str">
         <f t="shared" si="15"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 6092</v>
       </c>
       <c r="O72" t="str">
         <f t="shared" si="15"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 6092</v>
       </c>
       <c r="P72" t="str">
         <f t="shared" si="15"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
-      </c>
-    </row>
-    <row r="73" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 6092</v>
+      </c>
+      <c r="Q72" t="str">
+        <f t="shared" si="15"/>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 6092</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="11">
         <v>8500</v>
       </c>
@@ -4939,35 +4952,36 @@
         <f t="shared" si="20"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-2-2-1.xml</v>
       </c>
-      <c r="K73" t="str">
+      <c r="K73" s="13"/>
+      <c r="L73" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 8500</v>
       </c>
-      <c r="L73" t="str">
+      <c r="M73" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 8500</v>
       </c>
-      <c r="M73" t="str">
+      <c r="N73" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 8500</v>
       </c>
-      <c r="N73" t="str">
+      <c r="O73" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 8500</v>
       </c>
-      <c r="O73" t="str">
+      <c r="P73" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 8500</v>
       </c>
-      <c r="P73" t="str">
+      <c r="Q73" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 8500</v>
       </c>
-      <c r="Q73" s="13"/>
       <c r="R73" s="13"/>
       <c r="S73" s="13"/>
-    </row>
-    <row r="74" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="T73" s="13"/>
+    </row>
+    <row r="74" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="11">
         <v>5304</v>
       </c>
@@ -5003,32 +5017,32 @@
         <f t="shared" si="20"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-2-2-1.xml</v>
       </c>
-      <c r="K74" t="str">
+      <c r="L74" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 5304</v>
       </c>
-      <c r="L74" t="str">
+      <c r="M74" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 5304</v>
       </c>
-      <c r="M74" t="str">
+      <c r="N74" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 5304</v>
       </c>
-      <c r="N74" t="str">
+      <c r="O74" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 5304</v>
       </c>
-      <c r="O74" t="str">
+      <c r="P74" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 5304</v>
       </c>
-      <c r="P74" t="str">
+      <c r="Q74" t="str">
         <f t="shared" si="15"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 5304</v>
       </c>
     </row>
-    <row r="75" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>0</v>
       </c>
@@ -5061,32 +5075,32 @@
         <f t="shared" si="20"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-2-2-1.xml</v>
       </c>
-      <c r="K75" t="str">
+      <c r="L75" t="str">
         <f t="shared" si="15"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
       </c>
-      <c r="L75" t="str">
+      <c r="M75" t="str">
         <f t="shared" si="15"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
       </c>
-      <c r="M75" t="str">
+      <c r="N75" t="str">
         <f t="shared" si="15"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
       </c>
-      <c r="N75" t="str">
+      <c r="O75" t="str">
         <f t="shared" si="15"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
       </c>
-      <c r="O75" t="str">
+      <c r="P75" t="str">
         <f t="shared" si="15"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
       </c>
-      <c r="P75" t="str">
+      <c r="Q75" t="str">
         <f t="shared" si="15"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="76" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>0</v>
       </c>
@@ -5119,32 +5133,32 @@
         <f t="shared" si="20"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/500-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-2-2-1.xml</v>
       </c>
-      <c r="K76" t="str">
-        <f t="shared" ref="K76:P88" si="21">"zzz Infer "&amp;$A$2&amp;" "&amp;$F76&amp;" "&amp;K$2&amp;" "&amp;$A76</f>
+      <c r="L76" t="str">
+        <f t="shared" ref="L76:Q88" si="21">"zzz Infer "&amp;$A$2&amp;" "&amp;$F76&amp;" "&amp;L$2&amp;" "&amp;$A76</f>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
       </c>
-      <c r="L76" t="str">
+      <c r="M76" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
       </c>
-      <c r="M76" t="str">
+      <c r="N76" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
       </c>
-      <c r="N76" t="str">
+      <c r="O76" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
       </c>
-      <c r="O76" t="str">
+      <c r="P76" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
       </c>
-      <c r="P76" t="str">
+      <c r="Q76" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="77" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="11">
         <v>5776</v>
       </c>
@@ -5180,32 +5194,32 @@
         <f t="shared" si="20"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-2-2-1.xml</v>
       </c>
-      <c r="K77" t="str">
+      <c r="L77" t="str">
         <f t="shared" si="21"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 5776</v>
       </c>
-      <c r="L77" t="str">
+      <c r="M77" t="str">
         <f t="shared" si="21"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 5776</v>
       </c>
-      <c r="M77" t="str">
+      <c r="N77" t="str">
         <f t="shared" si="21"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 5776</v>
       </c>
-      <c r="N77" t="str">
+      <c r="O77" t="str">
         <f t="shared" si="21"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 5776</v>
       </c>
-      <c r="O77" t="str">
+      <c r="P77" t="str">
         <f t="shared" si="21"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 5776</v>
       </c>
-      <c r="P77" t="str">
+      <c r="Q77" t="str">
         <f t="shared" si="21"/>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 5776</v>
       </c>
     </row>
-    <row r="78" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>0</v>
       </c>
@@ -5238,32 +5252,32 @@
         <f t="shared" si="20"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-2-2-1.xml</v>
       </c>
-      <c r="K78" t="str">
+      <c r="L78" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
       </c>
-      <c r="L78" t="str">
+      <c r="M78" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
       </c>
-      <c r="M78" t="str">
+      <c r="N78" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
       </c>
-      <c r="N78" t="str">
+      <c r="O78" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
       </c>
-      <c r="O78" t="str">
+      <c r="P78" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
       </c>
-      <c r="P78" t="str">
+      <c r="Q78" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="79" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>0</v>
       </c>
@@ -5296,32 +5310,32 @@
         <f t="shared" si="20"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-2-2-1.xml</v>
       </c>
-      <c r="K79" t="str">
+      <c r="L79" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
       </c>
-      <c r="L79" t="str">
+      <c r="M79" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
       </c>
-      <c r="M79" t="str">
+      <c r="N79" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
       </c>
-      <c r="N79" t="str">
+      <c r="O79" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
       </c>
-      <c r="O79" t="str">
+      <c r="P79" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
       </c>
-      <c r="P79" t="str">
+      <c r="Q79" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="80" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>0</v>
       </c>
@@ -5354,32 +5368,32 @@
         <f t="shared" si="20"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/500-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-2-2-1.xml</v>
       </c>
-      <c r="K80" t="str">
+      <c r="L80" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
       </c>
-      <c r="L80" t="str">
+      <c r="M80" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
       </c>
-      <c r="M80" t="str">
+      <c r="N80" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
       </c>
-      <c r="N80" t="str">
+      <c r="O80" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
       </c>
-      <c r="O80" t="str">
+      <c r="P80" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
       </c>
-      <c r="P80" t="str">
+      <c r="Q80" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="81" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>0</v>
       </c>
@@ -5412,32 +5426,32 @@
         <f t="shared" si="20"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/SCGD-2-2-1.xml</v>
       </c>
-      <c r="K81" t="str">
+      <c r="L81" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
       </c>
-      <c r="L81" t="str">
+      <c r="M81" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
       </c>
-      <c r="M81" t="str">
+      <c r="N81" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
       </c>
-      <c r="N81" t="str">
+      <c r="O81" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
       </c>
-      <c r="O81" t="str">
+      <c r="P81" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
       </c>
-      <c r="P81" t="str">
+      <c r="Q81" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="82" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>0</v>
       </c>
@@ -5470,32 +5484,32 @@
         <f t="shared" si="20"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/SCGD-2-2-1.xml</v>
       </c>
-      <c r="K82" t="str">
+      <c r="L82" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
       </c>
-      <c r="L82" t="str">
+      <c r="M82" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
       </c>
-      <c r="M82" t="str">
+      <c r="N82" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
       </c>
-      <c r="N82" t="str">
+      <c r="O82" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
       </c>
-      <c r="O82" t="str">
+      <c r="P82" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
       </c>
-      <c r="P82" t="str">
+      <c r="Q82" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="83" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>0</v>
       </c>
@@ -5528,32 +5542,32 @@
         <f t="shared" si="20"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/SCGD-2-2-1.xml</v>
       </c>
-      <c r="K83" t="str">
+      <c r="L83" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
       </c>
-      <c r="L83" t="str">
+      <c r="M83" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
       </c>
-      <c r="M83" t="str">
+      <c r="N83" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
       </c>
-      <c r="N83" t="str">
+      <c r="O83" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
       </c>
-      <c r="O83" t="str">
+      <c r="P83" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
       </c>
-      <c r="P83" t="str">
+      <c r="Q83" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="84" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>0</v>
       </c>
@@ -5586,32 +5600,32 @@
         <f t="shared" si="20"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/500-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/SCGD-2-2-1.xml</v>
       </c>
-      <c r="K84" t="str">
+      <c r="L84" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
       </c>
-      <c r="L84" t="str">
+      <c r="M84" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
       </c>
-      <c r="M84" t="str">
+      <c r="N84" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
       </c>
-      <c r="N84" t="str">
+      <c r="O84" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
       </c>
-      <c r="O84" t="str">
+      <c r="P84" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
       </c>
-      <c r="P84" t="str">
+      <c r="Q84" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="85" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>0</v>
       </c>
@@ -5644,32 +5658,32 @@
         <f t="shared" si="20"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/SCGD-2-2-1.xml</v>
       </c>
-      <c r="K85" t="str">
+      <c r="L85" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
       </c>
-      <c r="L85" t="str">
+      <c r="M85" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
       </c>
-      <c r="M85" t="str">
+      <c r="N85" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
       </c>
-      <c r="N85" t="str">
+      <c r="O85" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
       </c>
-      <c r="O85" t="str">
+      <c r="P85" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
       </c>
-      <c r="P85" t="str">
+      <c r="Q85" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="86" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>0</v>
       </c>
@@ -5702,32 +5716,32 @@
         <f t="shared" si="20"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/SCGD-2-2-1.xml</v>
       </c>
-      <c r="K86" t="str">
+      <c r="L86" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
       </c>
-      <c r="L86" t="str">
+      <c r="M86" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
       </c>
-      <c r="M86" t="str">
+      <c r="N86" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
       </c>
-      <c r="N86" t="str">
+      <c r="O86" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
       </c>
-      <c r="O86" t="str">
+      <c r="P86" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
       </c>
-      <c r="P86" t="str">
+      <c r="Q86" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="87" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>0</v>
       </c>
@@ -5760,32 +5774,32 @@
         <f t="shared" si="20"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/SCGD-2-2-1.xml</v>
       </c>
-      <c r="K87" t="str">
+      <c r="L87" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
       </c>
-      <c r="L87" t="str">
+      <c r="M87" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
       </c>
-      <c r="M87" t="str">
+      <c r="N87" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
       </c>
-      <c r="N87" t="str">
+      <c r="O87" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
       </c>
-      <c r="O87" t="str">
+      <c r="P87" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
       </c>
-      <c r="P87" t="str">
+      <c r="Q87" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="88" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>0</v>
       </c>
@@ -5818,64 +5832,58 @@
         <f t="shared" si="20"/>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/500-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/SCGD-2-2-1.xml</v>
       </c>
-      <c r="K88" t="str">
+      <c r="L88" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
       </c>
-      <c r="L88" t="str">
+      <c r="M88" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
       </c>
-      <c r="M88" t="str">
+      <c r="N88" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
       </c>
-      <c r="N88" t="str">
+      <c r="O88" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
       </c>
-      <c r="O88" t="str">
+      <c r="P88" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
       </c>
-      <c r="P88" t="str">
+      <c r="Q88" t="str">
         <f t="shared" si="21"/>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="91" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="P91" t="s">
+    <row r="91" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q91" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="93" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="P93" t="s">
+    <row r="93" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q93" t="s">
         <v>46</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:S88">
+  <autoFilter ref="A4:T88">
     <filterColumn colId="1">
       <filters>
         <filter val="SCGD"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="2">
+    <filterColumn colId="3">
       <filters>
-        <filter val="1-1"/>
+        <filter val="06000"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="3">
+    <filterColumn colId="4">
       <filters>
-        <filter val="18000"/>
+        <filter val="200"/>
       </filters>
     </filterColumn>
-    <sortState ref="A5:T76">
-      <sortCondition descending="1" ref="B5:B76"/>
-      <sortCondition ref="E5:E76"/>
-      <sortCondition ref="C5:C76"/>
-      <sortCondition ref="D5:D76"/>
-    </sortState>
   </autoFilter>
   <sortState ref="A5:T88">
     <sortCondition descending="1" ref="B5:B88"/>

</xml_diff>

<commit_message>
created MemCheck Configuration. started working with VLD, and fixed the first few leaks
</commit_message>
<xml_diff>
--- a/TestSet21.xlsx
+++ b/TestSet21.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="53">
   <si>
     <t>SCGD</t>
   </si>
@@ -170,12 +170,6 @@
     <t>Config.NoInclude/DataSets/i0c-bsc1.xml</t>
   </si>
   <si>
-    <t>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 5764</t>
-  </si>
-  <si>
-    <t>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0a-bsc1.xml Config.NoInclude/Engines/SCGD-1-1.xml 5920</t>
-  </si>
-  <si>
     <t>Client XML:</t>
   </si>
   <si>
@@ -183,6 +177,18 @@
   </si>
   <si>
     <t>INS Infer Dataset</t>
+  </si>
+  <si>
+    <t>2-2-1Deep</t>
+  </si>
+  <si>
+    <t>12000</t>
+  </si>
+  <si>
+    <t>18000</t>
+  </si>
+  <si>
+    <t>24000</t>
   </si>
 </sst>
 </file>
@@ -232,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -263,6 +269,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -636,14 +645,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:T93"/>
+  <dimension ref="A1:T104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="4" topLeftCell="H38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="4" topLeftCell="F70" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="L74" sqref="L74"/>
+      <selection pane="bottomRight" activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,7 +679,7 @@
         <v>11</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>18</v>
@@ -786,7 +794,7 @@
         <v>i0c-bsc1.xml</v>
       </c>
     </row>
-    <row r="5" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
         <v>6556</v>
       </c>
@@ -851,7 +859,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 6556</v>
       </c>
     </row>
-    <row r="6" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>9048</v>
       </c>
@@ -916,7 +924,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 9048</v>
       </c>
     </row>
-    <row r="7" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>5368</v>
       </c>
@@ -984,7 +992,7 @@
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
     </row>
-    <row r="8" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1624</v>
       </c>
@@ -1049,7 +1057,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 1624</v>
       </c>
     </row>
-    <row r="9" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9368</v>
       </c>
@@ -1114,7 +1122,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 9368</v>
       </c>
     </row>
-    <row r="10" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3400</v>
       </c>
@@ -1179,7 +1187,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 3400</v>
       </c>
     </row>
-    <row r="11" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9372</v>
       </c>
@@ -1244,7 +1252,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 9372</v>
       </c>
     </row>
-    <row r="12" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3576</v>
       </c>
@@ -1309,7 +1317,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 3576</v>
       </c>
     </row>
-    <row r="13" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1980</v>
       </c>
@@ -1374,7 +1382,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 1980</v>
       </c>
     </row>
-    <row r="14" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>8052</v>
       </c>
@@ -1439,7 +1447,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 8052</v>
       </c>
     </row>
-    <row r="15" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>5532</v>
       </c>
@@ -1504,7 +1512,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 5532</v>
       </c>
     </row>
-    <row r="16" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>6348</v>
       </c>
@@ -1569,7 +1577,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 6348</v>
       </c>
     </row>
-    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>9488</v>
       </c>
@@ -1634,7 +1642,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 9488</v>
       </c>
     </row>
-    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4616</v>
       </c>
@@ -1699,7 +1707,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 4616</v>
       </c>
     </row>
-    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>7656</v>
       </c>
@@ -1764,7 +1772,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 7656</v>
       </c>
     </row>
-    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5340</v>
       </c>
@@ -1829,7 +1837,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 5340</v>
       </c>
     </row>
-    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="14">
         <v>9312</v>
       </c>
@@ -1894,7 +1902,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 9312</v>
       </c>
     </row>
-    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3144</v>
       </c>
@@ -1959,7 +1967,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 3144</v>
       </c>
     </row>
-    <row r="23" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>7688</v>
       </c>
@@ -2024,7 +2032,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 7688</v>
       </c>
     </row>
-    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3780</v>
       </c>
@@ -2089,7 +2097,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 3780</v>
       </c>
     </row>
-    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>796</v>
       </c>
@@ -2154,7 +2162,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 796</v>
       </c>
     </row>
-    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1340</v>
       </c>
@@ -2219,7 +2227,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 1340</v>
       </c>
     </row>
-    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>8896</v>
       </c>
@@ -2284,7 +2292,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 8896</v>
       </c>
     </row>
-    <row r="28" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>5656</v>
       </c>
@@ -2349,7 +2357,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 5656</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>2416</v>
       </c>
@@ -2414,7 +2422,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 2416</v>
       </c>
     </row>
-    <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>4696</v>
       </c>
@@ -2479,7 +2487,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 4696</v>
       </c>
     </row>
-    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>40</v>
       </c>
@@ -2544,7 +2552,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml MEM!</v>
       </c>
     </row>
-    <row r="32" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>7252</v>
       </c>
@@ -2609,7 +2617,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 7252</v>
       </c>
     </row>
-    <row r="33" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>4880</v>
       </c>
@@ -2674,7 +2682,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 4880</v>
       </c>
     </row>
-    <row r="34" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>40</v>
       </c>
@@ -2739,7 +2747,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml MEM!</v>
       </c>
     </row>
-    <row r="35" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3476</v>
       </c>
@@ -2804,7 +2812,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 3476</v>
       </c>
     </row>
-    <row r="36" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>3</v>
       </c>
@@ -2866,7 +2874,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="37" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="14" t="s">
         <v>3</v>
@@ -2932,7 +2940,7 @@
       <c r="S37" s="14"/>
       <c r="T37" s="14"/>
     </row>
-    <row r="38" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="14"/>
       <c r="B38" t="s">
         <v>3</v>
@@ -2995,7 +3003,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="39" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>3</v>
       </c>
@@ -3057,7 +3065,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="40" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>3</v>
       </c>
@@ -3119,7 +3127,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="41" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
         <v>5764</v>
       </c>
@@ -3184,7 +3192,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 5764</v>
       </c>
     </row>
-    <row r="42" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>5648</v>
       </c>
@@ -3249,7 +3257,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 5648</v>
       </c>
     </row>
-    <row r="43" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="10">
         <v>6176</v>
       </c>
@@ -3317,7 +3325,7 @@
       <c r="S43" s="10"/>
       <c r="T43" s="10"/>
     </row>
-    <row r="44" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B44" s="10" t="s">
         <v>0</v>
       </c>
@@ -3379,7 +3387,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="45" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>5356</v>
       </c>
@@ -3444,7 +3452,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 5356</v>
       </c>
     </row>
-    <row r="46" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>956</v>
       </c>
@@ -3509,7 +3517,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 956</v>
       </c>
     </row>
-    <row r="47" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>8195</v>
       </c>
@@ -3574,7 +3582,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 8195</v>
       </c>
     </row>
-    <row r="48" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>0</v>
       </c>
@@ -3636,7 +3644,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="49" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>8064</v>
       </c>
@@ -3701,7 +3709,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 8064</v>
       </c>
     </row>
-    <row r="50" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>6435</v>
       </c>
@@ -3766,7 +3774,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 6435</v>
       </c>
     </row>
-    <row r="51" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>7476</v>
       </c>
@@ -3831,7 +3839,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 7476</v>
       </c>
     </row>
-    <row r="52" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>0</v>
       </c>
@@ -3893,7 +3901,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="53" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>5212</v>
       </c>
@@ -3958,7 +3966,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 5212</v>
       </c>
     </row>
-    <row r="54" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>8636</v>
       </c>
@@ -4023,7 +4031,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 8636</v>
       </c>
     </row>
-    <row r="55" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="14">
         <v>8420</v>
       </c>
@@ -4091,7 +4099,7 @@
       <c r="S55" s="14"/>
       <c r="T55" s="14"/>
     </row>
-    <row r="56" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>0</v>
       </c>
@@ -4153,7 +4161,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="57" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <v>5920</v>
       </c>
@@ -4218,7 +4226,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 5920</v>
       </c>
     </row>
-    <row r="58" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>4935</v>
       </c>
@@ -4283,7 +4291,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 4935</v>
       </c>
     </row>
-    <row r="59" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>7360</v>
       </c>
@@ -4348,7 +4356,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 7360</v>
       </c>
     </row>
-    <row r="60" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2444</v>
       </c>
@@ -4413,7 +4421,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 2444</v>
       </c>
     </row>
-    <row r="61" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>6307</v>
       </c>
@@ -4478,7 +4486,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 6307</v>
       </c>
     </row>
-    <row r="62" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>6827</v>
       </c>
@@ -4543,7 +4551,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 6827</v>
       </c>
     </row>
-    <row r="63" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>7376</v>
       </c>
@@ -4608,7 +4616,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 7376</v>
       </c>
     </row>
-    <row r="64" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="14"/>
       <c r="B64" t="s">
         <v>0</v>
@@ -4671,7 +4679,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="65" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>8892</v>
       </c>
@@ -4736,7 +4744,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 8892</v>
       </c>
     </row>
-    <row r="66" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>6396</v>
       </c>
@@ -4801,7 +4809,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 6396</v>
       </c>
     </row>
-    <row r="67" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>7532</v>
       </c>
@@ -4866,7 +4874,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 7532</v>
       </c>
     </row>
-    <row r="68" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>0</v>
       </c>
@@ -4928,7 +4936,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="69" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>1212</v>
       </c>
@@ -4945,7 +4953,7 @@
         <v>39</v>
       </c>
       <c r="F69" t="str">
-        <f t="shared" ref="F69:F88" si="20">"Config.NoInclude/Client.xml"</f>
+        <f t="shared" ref="F69:F104" si="20">"Config.NoInclude/Client.xml"</f>
         <v>Config.NoInclude/Client.xml</v>
       </c>
       <c r="G69" t="str">
@@ -4953,15 +4961,15 @@
         <v>Config.NoInclude/DataShapes/050-1.xml</v>
       </c>
       <c r="H69" t="str">
-        <f t="shared" ref="H69:H88" si="22">"Config.NoInclude/Engines/"&amp;B69&amp;"-"&amp;C69&amp;".xml"</f>
+        <f t="shared" ref="H69:H89" si="22">"Config.NoInclude/Engines/"&amp;B69&amp;"-"&amp;C69&amp;".xml"</f>
         <v>Config.NoInclude/Engines/SCGD-1-1.xml</v>
       </c>
       <c r="I69" t="str">
-        <f t="shared" ref="I69:I88" si="23">"Config.NoInclude/DataSets/"&amp;D69&amp;".xml"</f>
+        <f t="shared" ref="I69:I92" si="23">"Config.NoInclude/DataSets/"&amp;D69&amp;".xml"</f>
         <v>Config.NoInclude/DataSets/24000.xml</v>
       </c>
       <c r="J69" t="str">
-        <f t="shared" ref="J69:J100" si="24">"zzz Both "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;G69&amp;" "&amp;I69&amp;" "&amp;H69</f>
+        <f t="shared" ref="J69:J88" si="24">"zzz Both "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;G69&amp;" "&amp;I69&amp;" "&amp;H69</f>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/SCGD-1-1.xml</v>
       </c>
       <c r="K69" s="14" t="str">
@@ -4993,7 +5001,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 1212</v>
       </c>
     </row>
-    <row r="70" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>5731</v>
       </c>
@@ -5058,7 +5066,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 5731</v>
       </c>
     </row>
-    <row r="71" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>5892</v>
       </c>
@@ -5123,7 +5131,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 5892</v>
       </c>
     </row>
-    <row r="72" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>6092</v>
       </c>
@@ -5321,7 +5329,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 5304</v>
       </c>
     </row>
-    <row r="75" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>0</v>
       </c>
@@ -5359,7 +5367,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-2-2-1.xml</v>
       </c>
       <c r="L75" t="str">
-        <f t="shared" ref="L75:Q88" si="26">"zzz Infer "&amp;$A$2&amp;" "&amp;$F75&amp;" "&amp;L$2&amp;" "&amp;$A75</f>
+        <f t="shared" ref="L75:Q90" si="26">"zzz Infer "&amp;$A$2&amp;" "&amp;$F75&amp;" "&amp;L$2&amp;" "&amp;$A75</f>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
       </c>
       <c r="M75" t="str">
@@ -5383,7 +5391,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="76" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>0</v>
       </c>
@@ -5578,7 +5586,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 984</v>
       </c>
     </row>
-    <row r="79" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" s="14"/>
       <c r="B79" t="s">
         <v>0</v>
@@ -5641,7 +5649,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="80" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>0</v>
       </c>
@@ -5703,7 +5711,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>3724</v>
       </c>
@@ -5768,7 +5776,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 3724</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" s="14">
         <v>9720</v>
       </c>
@@ -5833,7 +5841,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 9720</v>
       </c>
     </row>
-    <row r="83" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>0</v>
       </c>
@@ -5895,7 +5903,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="84" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>0</v>
       </c>
@@ -5957,7 +5965,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>0</v>
       </c>
@@ -6019,7 +6027,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>0</v>
       </c>
@@ -6081,7 +6089,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="87" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>0</v>
       </c>
@@ -6143,7 +6151,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="88" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>0</v>
       </c>
@@ -6205,41 +6213,1019 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="Q91" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="Q93" t="s">
-        <v>46</v>
-      </c>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>0</v>
+      </c>
+      <c r="C89" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D89" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E89" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F89" s="14" t="str">
+        <f t="shared" si="20"/>
+        <v>Config.NoInclude/Client.xml</v>
+      </c>
+      <c r="G89" s="14" t="str">
+        <f t="shared" ref="G89:G104" si="27">"Config.NoInclude/DataShapes/"&amp;E89&amp;"-"&amp;"1.xml"</f>
+        <v>Config.NoInclude/DataShapes/050-1.xml</v>
+      </c>
+      <c r="H89" s="14" t="str">
+        <f t="shared" ref="H89:H104" si="28">"Config.NoInclude/Engines/"&amp;B89&amp;"-"&amp;C89&amp;".xml"</f>
+        <v>Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="I89" s="14" t="str">
+        <f t="shared" ref="I89:I104" si="29">"Config.NoInclude/DataSets/"&amp;D89&amp;".xml"</f>
+        <v>Config.NoInclude/DataSets/06000.xml</v>
+      </c>
+      <c r="J89" s="14" t="str">
+        <f t="shared" ref="J89:J104" si="30">"zzz Both "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;G89&amp;" "&amp;I89&amp;" "&amp;H89</f>
+        <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="K89" s="14" t="str">
+        <f t="shared" ref="K89:K104" si="31">"zzz Infer "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;G89&amp;" "&amp;I89&amp;" "&amp;H89</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="L89" s="14" t="str">
+        <f t="shared" si="26"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
+      </c>
+      <c r="M89" s="14" t="str">
+        <f t="shared" si="26"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
+      </c>
+      <c r="N89" s="14" t="str">
+        <f t="shared" si="26"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
+      </c>
+      <c r="O89" s="14" t="str">
+        <f t="shared" si="26"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
+      </c>
+      <c r="P89" s="14" t="str">
+        <f t="shared" si="26"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
+      </c>
+      <c r="Q89" s="14" t="str">
+        <f t="shared" si="26"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
+      </c>
+      <c r="R89" s="14"/>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B90" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C90" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D90" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E90" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F90" s="14" t="str">
+        <f t="shared" si="20"/>
+        <v>Config.NoInclude/Client.xml</v>
+      </c>
+      <c r="G90" s="14" t="str">
+        <f t="shared" si="27"/>
+        <v>Config.NoInclude/DataShapes/050-1.xml</v>
+      </c>
+      <c r="H90" s="14" t="str">
+        <f t="shared" si="28"/>
+        <v>Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="I90" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>Config.NoInclude/DataSets/12000.xml</v>
+      </c>
+      <c r="J90" s="14" t="str">
+        <f t="shared" si="30"/>
+        <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="K90" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="L90" s="14" t="str">
+        <f t="shared" si="26"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
+      </c>
+      <c r="M90" s="14" t="str">
+        <f t="shared" si="26"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
+      </c>
+      <c r="N90" s="14" t="str">
+        <f t="shared" si="26"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
+      </c>
+      <c r="O90" s="14" t="str">
+        <f t="shared" si="26"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
+      </c>
+      <c r="P90" s="14" t="str">
+        <f t="shared" si="26"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
+      </c>
+      <c r="Q90" s="14" t="str">
+        <f t="shared" si="26"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
+      </c>
+      <c r="R90" s="14"/>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B91" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C91" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D91" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E91" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F91" s="14" t="str">
+        <f t="shared" si="20"/>
+        <v>Config.NoInclude/Client.xml</v>
+      </c>
+      <c r="G91" s="14" t="str">
+        <f t="shared" si="27"/>
+        <v>Config.NoInclude/DataShapes/050-1.xml</v>
+      </c>
+      <c r="H91" s="14" t="str">
+        <f t="shared" si="28"/>
+        <v>Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="I91" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>Config.NoInclude/DataSets/18000.xml</v>
+      </c>
+      <c r="J91" s="14" t="str">
+        <f t="shared" si="30"/>
+        <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="K91" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="L91" s="14" t="str">
+        <f t="shared" ref="L91:Q104" si="32">"zzz Infer "&amp;$A$2&amp;" "&amp;$F91&amp;" "&amp;L$2&amp;" "&amp;$A91</f>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
+      </c>
+      <c r="M91" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
+      </c>
+      <c r="N91" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
+      </c>
+      <c r="O91" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
+      </c>
+      <c r="P91" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
+      </c>
+      <c r="Q91" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
+      </c>
+      <c r="R91" s="14"/>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B92" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C92" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E92" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F92" s="14" t="str">
+        <f t="shared" si="20"/>
+        <v>Config.NoInclude/Client.xml</v>
+      </c>
+      <c r="G92" s="14" t="str">
+        <f t="shared" si="27"/>
+        <v>Config.NoInclude/DataShapes/050-1.xml</v>
+      </c>
+      <c r="H92" s="14" t="str">
+        <f t="shared" si="28"/>
+        <v>Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="I92" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>Config.NoInclude/DataSets/24000.xml</v>
+      </c>
+      <c r="J92" s="14" t="str">
+        <f t="shared" si="30"/>
+        <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="K92" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="L92" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
+      </c>
+      <c r="M92" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
+      </c>
+      <c r="N92" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
+      </c>
+      <c r="O92" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
+      </c>
+      <c r="P92" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
+      </c>
+      <c r="Q92" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
+      </c>
+      <c r="R92" s="14"/>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B93" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C93" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E93" s="6">
+        <v>100</v>
+      </c>
+      <c r="F93" s="14" t="str">
+        <f t="shared" si="20"/>
+        <v>Config.NoInclude/Client.xml</v>
+      </c>
+      <c r="G93" s="14" t="str">
+        <f t="shared" si="27"/>
+        <v>Config.NoInclude/DataShapes/100-1.xml</v>
+      </c>
+      <c r="H93" s="14" t="str">
+        <f t="shared" si="28"/>
+        <v>Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="I93" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>Config.NoInclude/DataSets/06000.xml</v>
+      </c>
+      <c r="J93" s="14" t="str">
+        <f t="shared" si="30"/>
+        <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="K93" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="L93" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
+      </c>
+      <c r="M93" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
+      </c>
+      <c r="N93" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
+      </c>
+      <c r="O93" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
+      </c>
+      <c r="P93" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
+      </c>
+      <c r="Q93" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
+      </c>
+      <c r="R93" s="14"/>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B94" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C94" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D94" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E94" s="6">
+        <v>100</v>
+      </c>
+      <c r="F94" s="14" t="str">
+        <f t="shared" si="20"/>
+        <v>Config.NoInclude/Client.xml</v>
+      </c>
+      <c r="G94" s="14" t="str">
+        <f t="shared" si="27"/>
+        <v>Config.NoInclude/DataShapes/100-1.xml</v>
+      </c>
+      <c r="H94" s="14" t="str">
+        <f t="shared" si="28"/>
+        <v>Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="I94" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>Config.NoInclude/DataSets/12000.xml</v>
+      </c>
+      <c r="J94" s="14" t="str">
+        <f t="shared" si="30"/>
+        <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="K94" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="L94" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
+      </c>
+      <c r="M94" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
+      </c>
+      <c r="N94" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
+      </c>
+      <c r="O94" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
+      </c>
+      <c r="P94" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
+      </c>
+      <c r="Q94" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
+      </c>
+      <c r="R94" s="14"/>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>8135</v>
+      </c>
+      <c r="B95" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C95" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D95" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E95" s="6">
+        <v>100</v>
+      </c>
+      <c r="F95" s="14" t="str">
+        <f t="shared" si="20"/>
+        <v>Config.NoInclude/Client.xml</v>
+      </c>
+      <c r="G95" s="14" t="str">
+        <f t="shared" si="27"/>
+        <v>Config.NoInclude/DataShapes/100-1.xml</v>
+      </c>
+      <c r="H95" s="14" t="str">
+        <f t="shared" si="28"/>
+        <v>Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="I95" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>Config.NoInclude/DataSets/18000.xml</v>
+      </c>
+      <c r="J95" s="14" t="str">
+        <f t="shared" si="30"/>
+        <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="K95" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="L95" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 8135</v>
+      </c>
+      <c r="M95" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 8135</v>
+      </c>
+      <c r="N95" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 8135</v>
+      </c>
+      <c r="O95" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 8135</v>
+      </c>
+      <c r="P95" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 8135</v>
+      </c>
+      <c r="Q95" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 8135</v>
+      </c>
+      <c r="R95" s="14"/>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B96" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C96" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D96" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E96" s="6">
+        <v>100</v>
+      </c>
+      <c r="F96" s="14" t="str">
+        <f t="shared" si="20"/>
+        <v>Config.NoInclude/Client.xml</v>
+      </c>
+      <c r="G96" s="14" t="str">
+        <f t="shared" si="27"/>
+        <v>Config.NoInclude/DataShapes/100-1.xml</v>
+      </c>
+      <c r="H96" s="14" t="str">
+        <f t="shared" si="28"/>
+        <v>Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="I96" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>Config.NoInclude/DataSets/24000.xml</v>
+      </c>
+      <c r="J96" s="14" t="str">
+        <f t="shared" si="30"/>
+        <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="K96" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="L96" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
+      </c>
+      <c r="M96" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
+      </c>
+      <c r="N96" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
+      </c>
+      <c r="O96" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
+      </c>
+      <c r="P96" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
+      </c>
+      <c r="Q96" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
+      </c>
+      <c r="R96" s="14"/>
+    </row>
+    <row r="97" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B97" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C97" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D97" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E97" s="6">
+        <v>200</v>
+      </c>
+      <c r="F97" s="14" t="str">
+        <f t="shared" si="20"/>
+        <v>Config.NoInclude/Client.xml</v>
+      </c>
+      <c r="G97" s="14" t="str">
+        <f t="shared" si="27"/>
+        <v>Config.NoInclude/DataShapes/200-1.xml</v>
+      </c>
+      <c r="H97" s="14" t="str">
+        <f t="shared" si="28"/>
+        <v>Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="I97" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>Config.NoInclude/DataSets/06000.xml</v>
+      </c>
+      <c r="J97" s="14" t="str">
+        <f t="shared" si="30"/>
+        <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="K97" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="L97" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
+      </c>
+      <c r="M97" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
+      </c>
+      <c r="N97" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
+      </c>
+      <c r="O97" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
+      </c>
+      <c r="P97" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
+      </c>
+      <c r="Q97" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
+      </c>
+      <c r="R97" s="14"/>
+    </row>
+    <row r="98" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B98" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C98" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D98" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E98" s="6">
+        <v>200</v>
+      </c>
+      <c r="F98" s="14" t="str">
+        <f t="shared" si="20"/>
+        <v>Config.NoInclude/Client.xml</v>
+      </c>
+      <c r="G98" s="14" t="str">
+        <f t="shared" si="27"/>
+        <v>Config.NoInclude/DataShapes/200-1.xml</v>
+      </c>
+      <c r="H98" s="14" t="str">
+        <f t="shared" si="28"/>
+        <v>Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="I98" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>Config.NoInclude/DataSets/12000.xml</v>
+      </c>
+      <c r="J98" s="14" t="str">
+        <f t="shared" si="30"/>
+        <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="K98" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="L98" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
+      </c>
+      <c r="M98" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
+      </c>
+      <c r="N98" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
+      </c>
+      <c r="O98" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
+      </c>
+      <c r="P98" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
+      </c>
+      <c r="Q98" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
+      </c>
+      <c r="R98" s="14"/>
+    </row>
+    <row r="99" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B99" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C99" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D99" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E99" s="6">
+        <v>200</v>
+      </c>
+      <c r="F99" s="14" t="str">
+        <f t="shared" si="20"/>
+        <v>Config.NoInclude/Client.xml</v>
+      </c>
+      <c r="G99" s="14" t="str">
+        <f t="shared" si="27"/>
+        <v>Config.NoInclude/DataShapes/200-1.xml</v>
+      </c>
+      <c r="H99" s="14" t="str">
+        <f t="shared" si="28"/>
+        <v>Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="I99" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>Config.NoInclude/DataSets/18000.xml</v>
+      </c>
+      <c r="J99" s="14" t="str">
+        <f t="shared" si="30"/>
+        <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="K99" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="L99" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
+      </c>
+      <c r="M99" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
+      </c>
+      <c r="N99" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
+      </c>
+      <c r="O99" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
+      </c>
+      <c r="P99" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
+      </c>
+      <c r="Q99" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
+      </c>
+      <c r="R99" s="14"/>
+    </row>
+    <row r="100" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B100" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C100" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D100" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E100" s="6">
+        <v>200</v>
+      </c>
+      <c r="F100" s="14" t="str">
+        <f t="shared" si="20"/>
+        <v>Config.NoInclude/Client.xml</v>
+      </c>
+      <c r="G100" s="14" t="str">
+        <f t="shared" si="27"/>
+        <v>Config.NoInclude/DataShapes/200-1.xml</v>
+      </c>
+      <c r="H100" s="14" t="str">
+        <f t="shared" si="28"/>
+        <v>Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="I100" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>Config.NoInclude/DataSets/24000.xml</v>
+      </c>
+      <c r="J100" s="14" t="str">
+        <f t="shared" si="30"/>
+        <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="K100" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="L100" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
+      </c>
+      <c r="M100" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
+      </c>
+      <c r="N100" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
+      </c>
+      <c r="O100" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
+      </c>
+      <c r="P100" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
+      </c>
+      <c r="Q100" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
+      </c>
+      <c r="R100" s="14"/>
+    </row>
+    <row r="101" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B101" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C101" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D101" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E101" s="6">
+        <v>500</v>
+      </c>
+      <c r="F101" s="14" t="str">
+        <f t="shared" si="20"/>
+        <v>Config.NoInclude/Client.xml</v>
+      </c>
+      <c r="G101" s="14" t="str">
+        <f t="shared" si="27"/>
+        <v>Config.NoInclude/DataShapes/500-1.xml</v>
+      </c>
+      <c r="H101" s="14" t="str">
+        <f t="shared" si="28"/>
+        <v>Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="I101" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>Config.NoInclude/DataSets/06000.xml</v>
+      </c>
+      <c r="J101" s="14" t="str">
+        <f t="shared" si="30"/>
+        <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/500-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="K101" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/500-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="L101" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
+      </c>
+      <c r="M101" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
+      </c>
+      <c r="N101" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
+      </c>
+      <c r="O101" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
+      </c>
+      <c r="P101" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
+      </c>
+      <c r="Q101" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
+      </c>
+      <c r="R101" s="14"/>
+    </row>
+    <row r="102" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B102" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C102" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D102" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E102" s="6">
+        <v>500</v>
+      </c>
+      <c r="F102" s="14" t="str">
+        <f t="shared" si="20"/>
+        <v>Config.NoInclude/Client.xml</v>
+      </c>
+      <c r="G102" s="14" t="str">
+        <f t="shared" si="27"/>
+        <v>Config.NoInclude/DataShapes/500-1.xml</v>
+      </c>
+      <c r="H102" s="14" t="str">
+        <f t="shared" si="28"/>
+        <v>Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="I102" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>Config.NoInclude/DataSets/12000.xml</v>
+      </c>
+      <c r="J102" s="14" t="str">
+        <f t="shared" si="30"/>
+        <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/500-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="K102" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/500-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="L102" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
+      </c>
+      <c r="M102" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
+      </c>
+      <c r="N102" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
+      </c>
+      <c r="O102" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
+      </c>
+      <c r="P102" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
+      </c>
+      <c r="Q102" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
+      </c>
+      <c r="R102" s="14"/>
+    </row>
+    <row r="103" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B103" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C103" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D103" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E103" s="6">
+        <v>500</v>
+      </c>
+      <c r="F103" s="14" t="str">
+        <f t="shared" si="20"/>
+        <v>Config.NoInclude/Client.xml</v>
+      </c>
+      <c r="G103" s="14" t="str">
+        <f t="shared" si="27"/>
+        <v>Config.NoInclude/DataShapes/500-1.xml</v>
+      </c>
+      <c r="H103" s="14" t="str">
+        <f t="shared" si="28"/>
+        <v>Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="I103" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>Config.NoInclude/DataSets/18000.xml</v>
+      </c>
+      <c r="J103" s="14" t="str">
+        <f t="shared" si="30"/>
+        <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/500-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="K103" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/500-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="L103" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
+      </c>
+      <c r="M103" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
+      </c>
+      <c r="N103" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
+      </c>
+      <c r="O103" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
+      </c>
+      <c r="P103" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
+      </c>
+      <c r="Q103" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
+      </c>
+      <c r="R103" s="14"/>
+    </row>
+    <row r="104" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B104" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C104" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D104" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E104" s="6">
+        <v>500</v>
+      </c>
+      <c r="F104" s="14" t="str">
+        <f t="shared" si="20"/>
+        <v>Config.NoInclude/Client.xml</v>
+      </c>
+      <c r="G104" s="14" t="str">
+        <f t="shared" si="27"/>
+        <v>Config.NoInclude/DataShapes/500-1.xml</v>
+      </c>
+      <c r="H104" s="14" t="str">
+        <f t="shared" si="28"/>
+        <v>Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="I104" s="14" t="str">
+        <f t="shared" si="29"/>
+        <v>Config.NoInclude/DataSets/24000.xml</v>
+      </c>
+      <c r="J104" s="14" t="str">
+        <f t="shared" si="30"/>
+        <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/500-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="K104" s="14" t="str">
+        <f t="shared" si="31"/>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/500-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+      </c>
+      <c r="L104" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
+      </c>
+      <c r="M104" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
+      </c>
+      <c r="N104" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
+      </c>
+      <c r="O104" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
+      </c>
+      <c r="P104" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
+      </c>
+      <c r="Q104" s="14" t="str">
+        <f t="shared" si="32"/>
+        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
+      </c>
+      <c r="R104" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:T88">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="SCGD"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="2-2-1"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="4">
-      <filters>
-        <filter val="100"/>
-        <filter val="050"/>
-      </filters>
-    </filterColumn>
-    <sortState ref="A5:T88">
-      <sortCondition descending="1" ref="B5:B88"/>
-      <sortCondition ref="C5:C88"/>
-      <sortCondition ref="D5:D88"/>
-      <sortCondition ref="E5:E88"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A4:T88"/>
   <sortState ref="A5:T88">
     <sortCondition descending="1" ref="B5:B88"/>
     <sortCondition ref="C5:C88"/>
@@ -6274,7 +7260,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B1" s="2">
         <v>21</v>
@@ -6293,7 +7279,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" s="15" t="str">
         <f t="shared" ref="B2" si="0">"Config.NoInclude/Client.xml"</f>

</xml_diff>

<commit_message>
fixed(?) bug in sCfgObj which tried to create the same debug file twice. Also, latest tests
</commit_message>
<xml_diff>
--- a/TestSet21.xlsx
+++ b/TestSet21.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="53">
   <si>
     <t>SCGD</t>
   </si>
@@ -189,18 +189,6 @@
   </si>
   <si>
     <t>24000</t>
-  </si>
-  <si>
-    <t>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 2416</t>
-  </si>
-  <si>
-    <t>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 4696</t>
-  </si>
-  <si>
-    <t>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 7252</t>
-  </si>
-  <si>
-    <t>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 3476</t>
   </si>
 </sst>
 </file>
@@ -658,13 +646,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:T110"/>
+  <dimension ref="A1:T104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="4" topLeftCell="J5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="O64" sqref="O64"/>
+      <selection pane="bottomRight" activeCell="J107" sqref="J107:J110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4434,7 +4422,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 2444</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>6307</v>
       </c>
@@ -4499,7 +4487,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 6307</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>6827</v>
       </c>
@@ -4564,7 +4552,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 6827</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>7376</v>
       </c>
@@ -4629,7 +4617,7 @@
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 7376</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="14"/>
       <c r="B64" t="s">
         <v>0</v>
@@ -6226,7 +6214,10 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
     </row>
-    <row r="89" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>10464</v>
+      </c>
       <c r="B89" t="s">
         <v>0</v>
       </c>
@@ -6240,56 +6231,59 @@
         <v>39</v>
       </c>
       <c r="F89" s="14" t="str">
-        <f t="shared" si="26"/>
+        <f>"Config.NoInclude/Client.xml"</f>
         <v>Config.NoInclude/Client.xml</v>
       </c>
       <c r="G89" s="14" t="str">
-        <f t="shared" ref="G89:G104" si="33">"Config.NoInclude/DataShapes/"&amp;E89&amp;"-"&amp;"1.xml"</f>
+        <f>"Config.NoInclude/DataShapes/"&amp;E89&amp;"-"&amp;"1.xml"</f>
         <v>Config.NoInclude/DataShapes/050-1.xml</v>
       </c>
       <c r="H89" s="14" t="str">
-        <f t="shared" ref="H89:H104" si="34">"Config.NoInclude/Engines/"&amp;B89&amp;"-"&amp;C89&amp;".xml"</f>
+        <f>"Config.NoInclude/Engines/"&amp;B89&amp;"-"&amp;C89&amp;".xml"</f>
         <v>Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
       </c>
       <c r="I89" s="14" t="str">
-        <f t="shared" ref="I89:I104" si="35">"Config.NoInclude/DataSets/"&amp;D89&amp;".xml"</f>
+        <f>"Config.NoInclude/DataSets/"&amp;D89&amp;".xml"</f>
         <v>Config.NoInclude/DataSets/06000.xml</v>
       </c>
       <c r="J89" s="14" t="str">
-        <f t="shared" ref="J89:J104" si="36">"zzz Both "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;G89&amp;" "&amp;I89&amp;" "&amp;H89</f>
+        <f>"zzz Both "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;G89&amp;" "&amp;I89&amp;" "&amp;H89</f>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
       </c>
       <c r="K89" s="14" t="str">
-        <f t="shared" ref="K89:K104" si="37">"zzz Infer "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;G89&amp;" "&amp;I89&amp;" "&amp;H89</f>
+        <f>"zzz Infer "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;G89&amp;" "&amp;I89&amp;" "&amp;H89</f>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
       </c>
       <c r="L89" s="14" t="str">
-        <f t="shared" si="32"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F89&amp;" "&amp;L$2&amp;" "&amp;$A89</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 10464</v>
       </c>
       <c r="M89" s="14" t="str">
-        <f t="shared" si="32"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F89&amp;" "&amp;M$2&amp;" "&amp;$A89</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 10464</v>
       </c>
       <c r="N89" s="14" t="str">
-        <f t="shared" si="32"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F89&amp;" "&amp;N$2&amp;" "&amp;$A89</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 10464</v>
       </c>
       <c r="O89" s="14" t="str">
-        <f t="shared" si="32"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F89&amp;" "&amp;O$2&amp;" "&amp;$A89</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 10464</v>
       </c>
       <c r="P89" s="14" t="str">
-        <f t="shared" si="32"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F89&amp;" "&amp;P$2&amp;" "&amp;$A89</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 10464</v>
       </c>
       <c r="Q89" s="14" t="str">
-        <f t="shared" si="32"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F89&amp;" "&amp;Q$2&amp;" "&amp;$A89</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 10464</v>
       </c>
       <c r="R89" s="14"/>
     </row>
-    <row r="90" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>3012</v>
+      </c>
       <c r="B90" s="14" t="s">
         <v>0</v>
       </c>
@@ -6297,62 +6291,65 @@
         <v>49</v>
       </c>
       <c r="D90" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E90" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="E90" s="6">
+        <v>100</v>
       </c>
       <c r="F90" s="14" t="str">
-        <f t="shared" si="26"/>
+        <f>"Config.NoInclude/Client.xml"</f>
         <v>Config.NoInclude/Client.xml</v>
       </c>
       <c r="G90" s="14" t="str">
-        <f t="shared" si="33"/>
-        <v>Config.NoInclude/DataShapes/050-1.xml</v>
+        <f>"Config.NoInclude/DataShapes/"&amp;E90&amp;"-"&amp;"1.xml"</f>
+        <v>Config.NoInclude/DataShapes/100-1.xml</v>
       </c>
       <c r="H90" s="14" t="str">
-        <f t="shared" si="34"/>
+        <f>"Config.NoInclude/Engines/"&amp;B90&amp;"-"&amp;C90&amp;".xml"</f>
         <v>Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
       </c>
       <c r="I90" s="14" t="str">
-        <f t="shared" si="35"/>
-        <v>Config.NoInclude/DataSets/12000.xml</v>
+        <f>"Config.NoInclude/DataSets/"&amp;D90&amp;".xml"</f>
+        <v>Config.NoInclude/DataSets/06000.xml</v>
       </c>
       <c r="J90" s="14" t="str">
-        <f t="shared" si="36"/>
-        <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+        <f>"zzz Both "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;G90&amp;" "&amp;I90&amp;" "&amp;H90</f>
+        <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
       </c>
       <c r="K90" s="14" t="str">
-        <f t="shared" si="37"/>
-        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+        <f>"zzz Infer "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;G90&amp;" "&amp;I90&amp;" "&amp;H90</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
       </c>
       <c r="L90" s="14" t="str">
-        <f t="shared" si="32"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F90&amp;" "&amp;L$2&amp;" "&amp;$A90</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 3012</v>
       </c>
       <c r="M90" s="14" t="str">
-        <f t="shared" si="32"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F90&amp;" "&amp;M$2&amp;" "&amp;$A90</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 3012</v>
       </c>
       <c r="N90" s="14" t="str">
-        <f t="shared" si="32"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F90&amp;" "&amp;N$2&amp;" "&amp;$A90</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 3012</v>
       </c>
       <c r="O90" s="14" t="str">
-        <f t="shared" si="32"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F90&amp;" "&amp;O$2&amp;" "&amp;$A90</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 3012</v>
       </c>
       <c r="P90" s="14" t="str">
-        <f t="shared" si="32"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F90&amp;" "&amp;P$2&amp;" "&amp;$A90</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 3012</v>
       </c>
       <c r="Q90" s="14" t="str">
-        <f t="shared" si="32"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F90&amp;" "&amp;Q$2&amp;" "&amp;$A90</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 3012</v>
       </c>
       <c r="R90" s="14"/>
     </row>
-    <row r="91" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>6560</v>
+      </c>
       <c r="B91" s="14" t="s">
         <v>0</v>
       </c>
@@ -6360,62 +6357,65 @@
         <v>49</v>
       </c>
       <c r="D91" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E91" s="7" t="s">
         <v>39</v>
       </c>
       <c r="F91" s="14" t="str">
-        <f t="shared" si="26"/>
+        <f>"Config.NoInclude/Client.xml"</f>
         <v>Config.NoInclude/Client.xml</v>
       </c>
       <c r="G91" s="14" t="str">
-        <f t="shared" si="33"/>
+        <f>"Config.NoInclude/DataShapes/"&amp;E91&amp;"-"&amp;"1.xml"</f>
         <v>Config.NoInclude/DataShapes/050-1.xml</v>
       </c>
       <c r="H91" s="14" t="str">
-        <f t="shared" si="34"/>
+        <f>"Config.NoInclude/Engines/"&amp;B91&amp;"-"&amp;C91&amp;".xml"</f>
         <v>Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
       </c>
       <c r="I91" s="14" t="str">
-        <f t="shared" si="35"/>
-        <v>Config.NoInclude/DataSets/18000.xml</v>
+        <f>"Config.NoInclude/DataSets/"&amp;D91&amp;".xml"</f>
+        <v>Config.NoInclude/DataSets/12000.xml</v>
       </c>
       <c r="J91" s="14" t="str">
-        <f t="shared" si="36"/>
-        <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+        <f>"zzz Both "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;G91&amp;" "&amp;I91&amp;" "&amp;H91</f>
+        <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
       </c>
       <c r="K91" s="14" t="str">
-        <f t="shared" si="37"/>
-        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+        <f>"zzz Infer "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;G91&amp;" "&amp;I91&amp;" "&amp;H91</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
       </c>
       <c r="L91" s="14" t="str">
-        <f t="shared" ref="L91:Q104" si="38">"zzz Infer "&amp;$A$2&amp;" "&amp;$F91&amp;" "&amp;L$2&amp;" "&amp;$A91</f>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F91&amp;" "&amp;L$2&amp;" "&amp;$A91</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 6560</v>
       </c>
       <c r="M91" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F91&amp;" "&amp;M$2&amp;" "&amp;$A91</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 6560</v>
       </c>
       <c r="N91" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F91&amp;" "&amp;N$2&amp;" "&amp;$A91</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 6560</v>
       </c>
       <c r="O91" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F91&amp;" "&amp;O$2&amp;" "&amp;$A91</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 6560</v>
       </c>
       <c r="P91" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F91&amp;" "&amp;P$2&amp;" "&amp;$A91</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 6560</v>
       </c>
       <c r="Q91" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F91&amp;" "&amp;Q$2&amp;" "&amp;$A91</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 6560</v>
       </c>
       <c r="R91" s="14"/>
     </row>
-    <row r="92" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>5371</v>
+      </c>
       <c r="B92" s="14" t="s">
         <v>0</v>
       </c>
@@ -6423,62 +6423,65 @@
         <v>49</v>
       </c>
       <c r="D92" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E92" s="7" t="s">
-        <v>39</v>
+        <v>50</v>
+      </c>
+      <c r="E92" s="6">
+        <v>100</v>
       </c>
       <c r="F92" s="14" t="str">
-        <f t="shared" si="26"/>
+        <f>"Config.NoInclude/Client.xml"</f>
         <v>Config.NoInclude/Client.xml</v>
       </c>
       <c r="G92" s="14" t="str">
-        <f t="shared" si="33"/>
-        <v>Config.NoInclude/DataShapes/050-1.xml</v>
+        <f>"Config.NoInclude/DataShapes/"&amp;E92&amp;"-"&amp;"1.xml"</f>
+        <v>Config.NoInclude/DataShapes/100-1.xml</v>
       </c>
       <c r="H92" s="14" t="str">
-        <f t="shared" si="34"/>
+        <f>"Config.NoInclude/Engines/"&amp;B92&amp;"-"&amp;C92&amp;".xml"</f>
         <v>Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
       </c>
       <c r="I92" s="14" t="str">
-        <f t="shared" si="35"/>
-        <v>Config.NoInclude/DataSets/24000.xml</v>
+        <f>"Config.NoInclude/DataSets/"&amp;D92&amp;".xml"</f>
+        <v>Config.NoInclude/DataSets/12000.xml</v>
       </c>
       <c r="J92" s="14" t="str">
-        <f t="shared" si="36"/>
-        <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+        <f>"zzz Both "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;G92&amp;" "&amp;I92&amp;" "&amp;H92</f>
+        <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
       </c>
       <c r="K92" s="14" t="str">
-        <f t="shared" si="37"/>
-        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+        <f>"zzz Infer "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;G92&amp;" "&amp;I92&amp;" "&amp;H92</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
       </c>
       <c r="L92" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F92&amp;" "&amp;L$2&amp;" "&amp;$A92</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 5371</v>
       </c>
       <c r="M92" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F92&amp;" "&amp;M$2&amp;" "&amp;$A92</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 5371</v>
       </c>
       <c r="N92" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F92&amp;" "&amp;N$2&amp;" "&amp;$A92</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 5371</v>
       </c>
       <c r="O92" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F92&amp;" "&amp;O$2&amp;" "&amp;$A92</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 5371</v>
       </c>
       <c r="P92" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F92&amp;" "&amp;P$2&amp;" "&amp;$A92</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 5371</v>
       </c>
       <c r="Q92" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F92&amp;" "&amp;Q$2&amp;" "&amp;$A92</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 5371</v>
       </c>
       <c r="R92" s="14"/>
     </row>
-    <row r="93" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>6012</v>
+      </c>
       <c r="B93" s="14" t="s">
         <v>0</v>
       </c>
@@ -6486,62 +6489,65 @@
         <v>49</v>
       </c>
       <c r="D93" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E93" s="6">
-        <v>100</v>
+        <v>51</v>
+      </c>
+      <c r="E93" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="F93" s="14" t="str">
-        <f t="shared" si="26"/>
+        <f>"Config.NoInclude/Client.xml"</f>
         <v>Config.NoInclude/Client.xml</v>
       </c>
       <c r="G93" s="14" t="str">
-        <f t="shared" si="33"/>
-        <v>Config.NoInclude/DataShapes/100-1.xml</v>
+        <f>"Config.NoInclude/DataShapes/"&amp;E93&amp;"-"&amp;"1.xml"</f>
+        <v>Config.NoInclude/DataShapes/050-1.xml</v>
       </c>
       <c r="H93" s="14" t="str">
-        <f t="shared" si="34"/>
+        <f>"Config.NoInclude/Engines/"&amp;B93&amp;"-"&amp;C93&amp;".xml"</f>
         <v>Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
       </c>
       <c r="I93" s="14" t="str">
-        <f t="shared" si="35"/>
-        <v>Config.NoInclude/DataSets/06000.xml</v>
+        <f>"Config.NoInclude/DataSets/"&amp;D93&amp;".xml"</f>
+        <v>Config.NoInclude/DataSets/18000.xml</v>
       </c>
       <c r="J93" s="14" t="str">
-        <f t="shared" si="36"/>
-        <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+        <f>"zzz Both "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;G93&amp;" "&amp;I93&amp;" "&amp;H93</f>
+        <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
       </c>
       <c r="K93" s="14" t="str">
-        <f t="shared" si="37"/>
-        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+        <f>"zzz Infer "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;G93&amp;" "&amp;I93&amp;" "&amp;H93</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
       </c>
       <c r="L93" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F93&amp;" "&amp;L$2&amp;" "&amp;$A93</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 6012</v>
       </c>
       <c r="M93" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F93&amp;" "&amp;M$2&amp;" "&amp;$A93</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 6012</v>
       </c>
       <c r="N93" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F93&amp;" "&amp;N$2&amp;" "&amp;$A93</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 6012</v>
       </c>
       <c r="O93" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F93&amp;" "&amp;O$2&amp;" "&amp;$A93</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 6012</v>
       </c>
       <c r="P93" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F93&amp;" "&amp;P$2&amp;" "&amp;$A93</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 6012</v>
       </c>
       <c r="Q93" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F93&amp;" "&amp;Q$2&amp;" "&amp;$A93</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 6012</v>
       </c>
       <c r="R93" s="14"/>
     </row>
-    <row r="94" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>8135</v>
+      </c>
       <c r="B94" s="14" t="s">
         <v>0</v>
       </c>
@@ -6549,64 +6555,64 @@
         <v>49</v>
       </c>
       <c r="D94" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E94" s="6">
         <v>100</v>
       </c>
       <c r="F94" s="14" t="str">
-        <f t="shared" si="26"/>
+        <f>"Config.NoInclude/Client.xml"</f>
         <v>Config.NoInclude/Client.xml</v>
       </c>
       <c r="G94" s="14" t="str">
-        <f t="shared" si="33"/>
+        <f>"Config.NoInclude/DataShapes/"&amp;E94&amp;"-"&amp;"1.xml"</f>
         <v>Config.NoInclude/DataShapes/100-1.xml</v>
       </c>
       <c r="H94" s="14" t="str">
-        <f t="shared" si="34"/>
+        <f>"Config.NoInclude/Engines/"&amp;B94&amp;"-"&amp;C94&amp;".xml"</f>
         <v>Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
       </c>
       <c r="I94" s="14" t="str">
-        <f t="shared" si="35"/>
-        <v>Config.NoInclude/DataSets/12000.xml</v>
+        <f>"Config.NoInclude/DataSets/"&amp;D94&amp;".xml"</f>
+        <v>Config.NoInclude/DataSets/18000.xml</v>
       </c>
       <c r="J94" s="14" t="str">
-        <f t="shared" si="36"/>
-        <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+        <f>"zzz Both "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;G94&amp;" "&amp;I94&amp;" "&amp;H94</f>
+        <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
       </c>
       <c r="K94" s="14" t="str">
-        <f t="shared" si="37"/>
-        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+        <f>"zzz Infer "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;G94&amp;" "&amp;I94&amp;" "&amp;H94</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
       </c>
       <c r="L94" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F94&amp;" "&amp;L$2&amp;" "&amp;$A94</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 8135</v>
       </c>
       <c r="M94" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F94&amp;" "&amp;M$2&amp;" "&amp;$A94</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 8135</v>
       </c>
       <c r="N94" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F94&amp;" "&amp;N$2&amp;" "&amp;$A94</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 8135</v>
       </c>
       <c r="O94" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F94&amp;" "&amp;O$2&amp;" "&amp;$A94</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 8135</v>
       </c>
       <c r="P94" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F94&amp;" "&amp;P$2&amp;" "&amp;$A94</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 8135</v>
       </c>
       <c r="Q94" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F94&amp;" "&amp;Q$2&amp;" "&amp;$A94</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 8135</v>
       </c>
       <c r="R94" s="14"/>
     </row>
-    <row r="95" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>8135</v>
+        <v>7483</v>
       </c>
       <c r="B95" s="14" t="s">
         <v>0</v>
@@ -6615,62 +6621,65 @@
         <v>49</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E95" s="6">
-        <v>100</v>
+        <v>52</v>
+      </c>
+      <c r="E95" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="F95" s="14" t="str">
-        <f t="shared" si="26"/>
+        <f>"Config.NoInclude/Client.xml"</f>
         <v>Config.NoInclude/Client.xml</v>
       </c>
       <c r="G95" s="14" t="str">
-        <f t="shared" si="33"/>
-        <v>Config.NoInclude/DataShapes/100-1.xml</v>
+        <f>"Config.NoInclude/DataShapes/"&amp;E95&amp;"-"&amp;"1.xml"</f>
+        <v>Config.NoInclude/DataShapes/050-1.xml</v>
       </c>
       <c r="H95" s="14" t="str">
-        <f t="shared" si="34"/>
+        <f>"Config.NoInclude/Engines/"&amp;B95&amp;"-"&amp;C95&amp;".xml"</f>
         <v>Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
       </c>
       <c r="I95" s="14" t="str">
-        <f t="shared" si="35"/>
-        <v>Config.NoInclude/DataSets/18000.xml</v>
+        <f>"Config.NoInclude/DataSets/"&amp;D95&amp;".xml"</f>
+        <v>Config.NoInclude/DataSets/24000.xml</v>
       </c>
       <c r="J95" s="14" t="str">
-        <f t="shared" si="36"/>
-        <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+        <f>"zzz Both "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;G95&amp;" "&amp;I95&amp;" "&amp;H95</f>
+        <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
       </c>
       <c r="K95" s="14" t="str">
-        <f t="shared" si="37"/>
-        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
+        <f>"zzz Infer "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;G95&amp;" "&amp;I95&amp;" "&amp;H95</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
       </c>
       <c r="L95" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 8135</v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F95&amp;" "&amp;L$2&amp;" "&amp;$A95</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml 7483</v>
       </c>
       <c r="M95" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 8135</v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F95&amp;" "&amp;M$2&amp;" "&amp;$A95</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml 7483</v>
       </c>
       <c r="N95" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 8135</v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F95&amp;" "&amp;N$2&amp;" "&amp;$A95</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml 7483</v>
       </c>
       <c r="O95" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 8135</v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F95&amp;" "&amp;O$2&amp;" "&amp;$A95</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml 7483</v>
       </c>
       <c r="P95" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 8135</v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F95&amp;" "&amp;P$2&amp;" "&amp;$A95</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml 7483</v>
       </c>
       <c r="Q95" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 8135</v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F95&amp;" "&amp;Q$2&amp;" "&amp;$A95</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml 7483</v>
       </c>
       <c r="R95" s="14"/>
     </row>
-    <row r="96" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>40</v>
+      </c>
       <c r="B96" s="14" t="s">
         <v>0</v>
       </c>
@@ -6684,52 +6693,52 @@
         <v>100</v>
       </c>
       <c r="F96" s="14" t="str">
-        <f t="shared" si="26"/>
+        <f>"Config.NoInclude/Client.xml"</f>
         <v>Config.NoInclude/Client.xml</v>
       </c>
       <c r="G96" s="14" t="str">
-        <f t="shared" si="33"/>
+        <f>"Config.NoInclude/DataShapes/"&amp;E96&amp;"-"&amp;"1.xml"</f>
         <v>Config.NoInclude/DataShapes/100-1.xml</v>
       </c>
       <c r="H96" s="14" t="str">
-        <f t="shared" si="34"/>
+        <f>"Config.NoInclude/Engines/"&amp;B96&amp;"-"&amp;C96&amp;".xml"</f>
         <v>Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
       </c>
       <c r="I96" s="14" t="str">
-        <f t="shared" si="35"/>
+        <f>"Config.NoInclude/DataSets/"&amp;D96&amp;".xml"</f>
         <v>Config.NoInclude/DataSets/24000.xml</v>
       </c>
       <c r="J96" s="14" t="str">
-        <f t="shared" si="36"/>
+        <f>"zzz Both "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;G96&amp;" "&amp;I96&amp;" "&amp;H96</f>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
       </c>
       <c r="K96" s="14" t="str">
-        <f t="shared" si="37"/>
+        <f>"zzz Infer "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;G96&amp;" "&amp;I96&amp;" "&amp;H96</f>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/24000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
       </c>
       <c r="L96" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F96&amp;" "&amp;L$2&amp;" "&amp;$A96</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml MEM!</v>
       </c>
       <c r="M96" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F96&amp;" "&amp;M$2&amp;" "&amp;$A96</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i1.xml MEM!</v>
       </c>
       <c r="N96" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F96&amp;" "&amp;N$2&amp;" "&amp;$A96</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i2.xml MEM!</v>
       </c>
       <c r="O96" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F96&amp;" "&amp;O$2&amp;" "&amp;$A96</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0a.xml MEM!</v>
       </c>
       <c r="P96" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F96&amp;" "&amp;P$2&amp;" "&amp;$A96</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0b.xml MEM!</v>
       </c>
       <c r="Q96" s="14" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
+        <f>"zzz Infer "&amp;$A$2&amp;" "&amp;$F96&amp;" "&amp;Q$2&amp;" "&amp;$A96</f>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml MEM!</v>
       </c>
       <c r="R96" s="14"/>
     </row>
@@ -6751,27 +6760,27 @@
         <v>Config.NoInclude/Client.xml</v>
       </c>
       <c r="G97" s="14" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" ref="G89:G104" si="33">"Config.NoInclude/DataShapes/"&amp;E97&amp;"-"&amp;"1.xml"</f>
         <v>Config.NoInclude/DataShapes/200-1.xml</v>
       </c>
       <c r="H97" s="14" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" ref="H89:H104" si="34">"Config.NoInclude/Engines/"&amp;B97&amp;"-"&amp;C97&amp;".xml"</f>
         <v>Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
       </c>
       <c r="I97" s="14" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" ref="I89:I104" si="35">"Config.NoInclude/DataSets/"&amp;D97&amp;".xml"</f>
         <v>Config.NoInclude/DataSets/06000.xml</v>
       </c>
       <c r="J97" s="14" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" ref="J89:J104" si="36">"zzz Both "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;G97&amp;" "&amp;I97&amp;" "&amp;H97</f>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
       </c>
       <c r="K97" s="14" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" ref="K89:K104" si="37">"zzz Infer "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;G97&amp;" "&amp;I97&amp;" "&amp;H97</f>
         <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-2-2-1Deep.xml</v>
       </c>
       <c r="L97" s="14" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" ref="L91:Q104" si="38">"zzz Infer "&amp;$A$2&amp;" "&amp;$F97&amp;" "&amp;L$2&amp;" "&amp;$A97</f>
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0.xml </v>
       </c>
       <c r="M97" s="14" t="str">
@@ -7236,26 +7245,6 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataSets/i0c.xml </v>
       </c>
       <c r="R104" s="14"/>
-    </row>
-    <row r="107" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="J107" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="108" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="J108" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="109" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="J109" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="110" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="J110" t="s">
-        <v>56</v>
-      </c>
     </row>
   </sheetData>
   <autoFilter ref="A4:T104">
@@ -7266,16 +7255,18 @@
     </filterColumn>
     <filterColumn colId="2">
       <filters>
-        <filter val="1-1"/>
+        <filter val="2-2-1Deep"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="3">
+    <filterColumn colId="4">
       <filters>
-        <filter val="12000"/>
+        <filter val="100"/>
+        <filter val="050"/>
       </filters>
     </filterColumn>
-    <sortState ref="A5:T16">
+    <sortState ref="A89:T96">
       <sortCondition ref="D5:D104"/>
+      <sortCondition ref="G5:G104"/>
       <sortCondition ref="E5:E104"/>
     </sortState>
   </autoFilter>

</xml_diff>